<commit_message>
extracted excel parsing from HasmParser
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Full with microinstruction" sheetId="3" r:id="rId1"/>
+    <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
     <sheet name="Encoding" sheetId="1" r:id="rId2"/>
-    <sheet name="Summary" sheetId="2" r:id="rId3"/>
+    <sheet name="Operands" sheetId="5" r:id="rId3"/>
+    <sheet name="Summary" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="300">
   <si>
     <t>Instruction</t>
   </si>
@@ -866,30 +867,6 @@
     <t>SPC = IMM12</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">TOS &lt;- PC + </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>, PC &lt;- IMM8</t>
-    </r>
-  </si>
-  <si>
     <t>if ccc = 1 PC = PC + IMM8</t>
   </si>
   <si>
@@ -930,6 +907,57 @@
   </si>
   <si>
     <t>SPC &lt;- TOS</t>
+  </si>
+  <si>
+    <t>r0</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>r4</t>
+  </si>
+  <si>
+    <t>r5</t>
+  </si>
+  <si>
+    <t>r6</t>
+  </si>
+  <si>
+    <t>r7</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>DST,REG,REG1</t>
+  </si>
+  <si>
+    <t>Constant</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Operand</t>
+  </si>
+  <si>
+    <t>Bits</t>
+  </si>
+  <si>
+    <t>SRC,REG2</t>
+  </si>
+  <si>
+    <t>Encoding Mask</t>
   </si>
 </sst>
 </file>
@@ -1691,1636 +1719,1149 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.5" style="17" customWidth="1"/>
-    <col min="4" max="4" width="2.125" customWidth="1"/>
-    <col min="5" max="5" width="25.25" style="17" customWidth="1"/>
-    <col min="6" max="6" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.375" customWidth="1"/>
-    <col min="8" max="8" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.375" customWidth="1"/>
+    <col min="2" max="2" width="25.25" style="17" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" customWidth="1"/>
+    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
     <col min="10" max="10" width="3.25" customWidth="1"/>
     <col min="11" max="11" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>1</v>
+        <v>238</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35" t="s">
-        <v>238</v>
-      </c>
-      <c r="F1" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>239</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="E1" s="36" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19" t="s">
+      <c r="B2" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="H2" s="23">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="B3" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="H3" s="23">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="32" t="s">
+      <c r="B4" s="32" t="s">
         <v>218</v>
       </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H4" s="33">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32" t="s">
+      <c r="B5" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H5" s="33">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="32" t="s">
+      <c r="B6" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H6" s="33">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E6" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32" t="s">
+      <c r="B7" s="32" t="s">
         <v>221</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H7" s="33">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32" t="s">
+      <c r="B8" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H8" s="33">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E8" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32" t="s">
+      <c r="B9" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H9" s="33">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E9" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="32" t="s">
+      <c r="B10" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H10" s="33">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32" t="s">
+      <c r="B11" s="32" t="s">
         <v>224</v>
       </c>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H11" s="33">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E11" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32" t="s">
+      <c r="B12" s="32" t="s">
         <v>226</v>
       </c>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H12" s="33">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E12" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32" t="s">
+      <c r="B13" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H13" s="33">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E13" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32" t="s">
+      <c r="B14" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H14" s="33">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32" t="s">
+      <c r="B15" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H15" s="33">
+      <c r="C15" s="31"/>
+      <c r="D15" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32" t="s">
+      <c r="B16" s="32" t="s">
         <v>229</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H16" s="33">
+      <c r="C16" s="31"/>
+      <c r="D16" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E16" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32" t="s">
+      <c r="B17" s="32" t="s">
         <v>230</v>
       </c>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H17" s="33">
+      <c r="C17" s="31"/>
+      <c r="D17" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E17" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32" t="s">
+      <c r="B18" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H18" s="33">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E18" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32" t="s">
+      <c r="B19" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H19" s="33">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E19" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="B20" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32" t="s">
+      <c r="B20" s="32" t="s">
         <v>233</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H20" s="33">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E20" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="B21" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32" t="s">
+      <c r="B21" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H21" s="33">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E21" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32" t="s">
+      <c r="B22" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H22" s="33">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E22" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="19" t="s">
+      <c r="B23" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="H23" s="23">
+      <c r="C23" s="18"/>
+      <c r="D23" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E23" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>75</v>
-      </c>
+      <c r="B24" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C24" s="18"/>
       <c r="D24" s="18"/>
-      <c r="E24" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E24" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="26" t="s">
+      <c r="B25" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="C25" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="G25" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D25" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>78</v>
+      <c r="B26" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="D26" s="18"/>
-      <c r="E26" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="G26" s="18"/>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E26" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="26" t="s">
+      <c r="B27" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H27" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="25"/>
+      <c r="D27" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E27" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C28" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="31"/>
-      <c r="E28" s="32" t="s">
+      <c r="B28" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H28" s="33">
+      <c r="C28" s="31"/>
+      <c r="D28" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E28" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="32" t="s">
+      <c r="B29" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H29" s="33">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E29" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="31" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="D30" s="31"/>
-      <c r="E30" s="32" t="s">
+      <c r="B30" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H30" s="33">
+      <c r="C30" s="31"/>
+      <c r="D30" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E30" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32" t="s">
+      <c r="B31" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H31" s="33">
+      <c r="C31" s="31"/>
+      <c r="D31" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E31" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="D32" s="31"/>
-      <c r="E32" s="32" t="s">
+      <c r="B32" s="32" t="s">
         <v>253</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H32" s="33">
+      <c r="C32" s="31"/>
+      <c r="D32" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E32" s="33">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
         <v>197</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>191</v>
+      <c r="B33" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="D33" s="18"/>
-      <c r="E33" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="G33" s="18"/>
-      <c r="H33" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E33" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="26" t="s">
+      <c r="B34" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H34" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="25"/>
+      <c r="D34" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E34" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>67</v>
+      <c r="B35" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="D35" s="18"/>
-      <c r="E35" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E35" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="26" t="s">
+      <c r="B36" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H36" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="25"/>
+      <c r="D36" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E36" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>198</v>
       </c>
-      <c r="B37" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C37" s="19" t="s">
-        <v>192</v>
-      </c>
+      <c r="B37" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C37" s="18"/>
       <c r="D37" s="18"/>
-      <c r="E37" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E37" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="26" t="s">
+      <c r="B38" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="F38" s="25" t="s">
+      <c r="C38" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="G38" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H38" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E38" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="C39" s="19" t="s">
-        <v>71</v>
-      </c>
+      <c r="B39" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C39" s="18"/>
       <c r="D39" s="18"/>
-      <c r="E39" s="19" t="s">
-        <v>247</v>
-      </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E39" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="26" t="s">
+      <c r="B40" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="F40" s="25" t="s">
+      <c r="C40" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="G40" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H40" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D40" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E40" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="C41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="20"/>
       <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="29"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E41" s="29"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="B42" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>193</v>
+      <c r="B42" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="D42" s="18"/>
-      <c r="E42" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="F42" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="G42" s="18"/>
-      <c r="H42" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E42" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="26" t="s">
+      <c r="B43" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H43" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="25"/>
+      <c r="D43" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E43" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="19" t="s">
-        <v>89</v>
+      <c r="B44" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="D44" s="18"/>
-      <c r="E44" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="G44" s="18"/>
-      <c r="H44" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E44" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="24"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="26" t="s">
+      <c r="B45" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H45" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="25"/>
+      <c r="D45" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E45" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="19" t="s">
-        <v>93</v>
-      </c>
+      <c r="B46" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C46" s="18"/>
       <c r="D46" s="18"/>
-      <c r="E46" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E46" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="26" t="s">
+      <c r="B47" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="F47" s="25" t="s">
+      <c r="C47" s="25" t="s">
         <v>244</v>
       </c>
-      <c r="G47" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H47" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D47" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E47" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>96</v>
+      <c r="B48" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="D48" s="18"/>
-      <c r="E48" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="G48" s="18"/>
-      <c r="H48" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E48" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="24"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="26" t="s">
+      <c r="B49" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H49" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="25"/>
+      <c r="D49" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C50" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D50" s="31"/>
-      <c r="E50" s="32" t="s">
+      <c r="B50" s="32" t="s">
         <v>257</v>
       </c>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H50" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="31"/>
+      <c r="D50" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E50" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C51" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D51" s="31"/>
-      <c r="E51" s="32" t="s">
+      <c r="B51" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="F51" s="31"/>
-      <c r="G51" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H51" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="31"/>
+      <c r="D51" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E51" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C52" s="19" t="s">
-        <v>269</v>
-      </c>
+      <c r="B52" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C52" s="18"/>
       <c r="D52" s="18"/>
-      <c r="E52" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="F52" s="18"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E52" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="21"/>
+      <c r="B53" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C53" s="20"/>
       <c r="D53" s="20"/>
-      <c r="E53" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E53" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="26" t="s">
+      <c r="B54" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H54" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="25"/>
+      <c r="D54" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E54" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>152</v>
       </c>
-      <c r="B55" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>50</v>
-      </c>
+      <c r="B55" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55" s="18"/>
       <c r="D55" s="18"/>
-      <c r="E55" s="19" t="s">
-        <v>241</v>
-      </c>
-      <c r="F55" s="18"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E55" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="28"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="21"/>
+      <c r="B56" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C56" s="20"/>
       <c r="D56" s="20"/>
-      <c r="E56" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E56" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="26" t="s">
+      <c r="B57" s="26" t="s">
         <v>258</v>
       </c>
-      <c r="F57" s="25"/>
-      <c r="G57" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H57" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="25"/>
+      <c r="D57" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E57" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>59</v>
+      <c r="B58" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>245</v>
       </c>
       <c r="D58" s="18"/>
-      <c r="E58" s="19" t="s">
-        <v>240</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="G58" s="18"/>
-      <c r="H58" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E58" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="25"/>
-      <c r="E59" s="26" t="s">
+      <c r="B59" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="F59" s="25"/>
-      <c r="G59" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="H59" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="25"/>
+      <c r="D59" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="E59" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="B60" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="C60" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="D60" s="31"/>
-      <c r="E60" s="32" t="s">
+      <c r="B60" s="32" t="s">
         <v>264</v>
       </c>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H60" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="31"/>
+      <c r="D60" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E60" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>158</v>
       </c>
-      <c r="B61" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="C61" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H61" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="C61" s="31"/>
+      <c r="D61" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E61" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="31" t="s">
-        <v>161</v>
-      </c>
-      <c r="C62" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D62" s="31"/>
-      <c r="E62" s="32" t="s">
+      <c r="B62" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="F62" s="31"/>
-      <c r="G62" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H62" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="31"/>
+      <c r="D62" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E62" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="B63" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="C63" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H63" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="C63" s="31"/>
+      <c r="D63" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E63" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="B64" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="C64" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="D64" s="31"/>
-      <c r="E64" s="32" t="s">
+      <c r="B64" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H64" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C64" s="31"/>
+      <c r="D64" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E64" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="B65" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D65" s="31"/>
-      <c r="E65" s="32" t="s">
-        <v>271</v>
-      </c>
-      <c r="F65" s="31"/>
-      <c r="G65" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H65" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="C65" s="31"/>
+      <c r="D65" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E65" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="B66" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="C66" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="D66" s="31"/>
-      <c r="E66" s="32" t="s">
-        <v>272</v>
-      </c>
-      <c r="F66" s="31"/>
-      <c r="G66" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H66" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="C66" s="31"/>
+      <c r="D66" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E66" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="B67" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C67" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="D67" s="31"/>
-      <c r="E67" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H67" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="C67" s="31"/>
+      <c r="D67" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E67" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="B68" s="31" t="s">
-        <v>171</v>
-      </c>
-      <c r="C68" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="D68" s="31"/>
-      <c r="E68" s="32" t="s">
-        <v>274</v>
-      </c>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H68" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E68" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="B69" s="31" t="s">
-        <v>175</v>
-      </c>
-      <c r="C69" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="D69" s="31"/>
-      <c r="E69" s="32" t="s">
-        <v>275</v>
-      </c>
-      <c r="F69" s="31"/>
-      <c r="G69" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H69" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="C69" s="31"/>
+      <c r="D69" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E69" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="B70" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="C70" s="32" t="s">
-        <v>180</v>
-      </c>
-      <c r="D70" s="31"/>
-      <c r="E70" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="F70" s="31"/>
-      <c r="G70" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H70" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="C70" s="31"/>
+      <c r="D70" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E70" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="B71" s="31" t="s">
-        <v>179</v>
-      </c>
-      <c r="C71" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="D71" s="31"/>
-      <c r="E71" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H71" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C71" s="31"/>
+      <c r="D71" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E71" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>183</v>
       </c>
-      <c r="B72" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="C72" s="32" t="s">
-        <v>185</v>
-      </c>
-      <c r="D72" s="31"/>
-      <c r="E72" s="32" t="s">
-        <v>278</v>
-      </c>
-      <c r="F72" s="31"/>
-      <c r="G72" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H72" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C72" s="31"/>
+      <c r="D72" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E72" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="B73" s="31" t="s">
-        <v>187</v>
-      </c>
-      <c r="C73" s="32" t="s">
-        <v>184</v>
-      </c>
-      <c r="D73" s="31"/>
-      <c r="E73" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H73" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="C73" s="31"/>
+      <c r="D73" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E73" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="B74" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="C74" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="D74" s="31"/>
-      <c r="E74" s="32" t="s">
+      <c r="B74" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="F74" s="31"/>
-      <c r="G74" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H74" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="31"/>
+      <c r="D74" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E74" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="B75" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="C75" s="32" t="s">
-        <v>209</v>
-      </c>
-      <c r="D75" s="31"/>
-      <c r="E75" s="32" t="s">
+      <c r="B75" s="32" t="s">
         <v>266</v>
       </c>
-      <c r="F75" s="31"/>
-      <c r="G75" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H75" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="31"/>
+      <c r="D75" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E75" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="B76" s="31" t="s">
-        <v>210</v>
-      </c>
-      <c r="C76" s="32" t="s">
-        <v>211</v>
-      </c>
-      <c r="D76" s="31"/>
-      <c r="E76" s="32" t="s">
+      <c r="B76" s="32" t="s">
         <v>267</v>
       </c>
-      <c r="F76" s="31"/>
-      <c r="G76" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H76" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="31"/>
+      <c r="D76" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E76" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="B77" s="31" t="s">
-        <v>213</v>
-      </c>
-      <c r="C77" s="32" t="s">
-        <v>214</v>
-      </c>
-      <c r="D77" s="31"/>
-      <c r="E77" s="32" t="s">
+      <c r="B77" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="F77" s="31"/>
-      <c r="G77" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H77" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C77" s="31"/>
+      <c r="D77" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E77" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>188</v>
       </c>
-      <c r="B78" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="C78" s="32" t="s">
+      <c r="B78" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="D78" s="31"/>
-      <c r="E78" s="32" t="s">
-        <v>188</v>
-      </c>
-      <c r="F78" s="31"/>
-      <c r="G78" s="31" t="s">
-        <v>237</v>
-      </c>
-      <c r="H78" s="33">
+      <c r="C78" s="31"/>
+      <c r="D78" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E78" s="33">
         <v>0</v>
       </c>
     </row>
@@ -4214,13 +3755,13 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>150</v>
@@ -4231,13 +3772,13 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>150</v>
@@ -4816,9 +4357,194 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="4.625" customWidth="1"/>
+    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>285</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>287</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>289</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" t="s">
+        <v>292</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>283</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>285</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>286</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>287</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>288</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>289</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>290</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
operand registers parsing from excel sheet
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Dropbox\LT Project\Architectuur\rev3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Documents\Programming\C#\Language\HomebrewAssembler\HasmParser\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
@@ -2874,8 +2874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4359,7 +4359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
parses immediates, range not taken in account yet
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Documents\Programming\C#\Language\HomebrewAssembler\HasmParser\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Documents\Programming\C#\Language\hasm\HasmParser\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="309">
   <si>
     <t>Instruction</t>
   </si>
@@ -942,9 +942,6 @@
     <t>DST,REG,REG1</t>
   </si>
   <si>
-    <t>Constant</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
@@ -958,6 +955,36 @@
   </si>
   <si>
     <t>Encoding Mask</t>
+  </si>
+  <si>
+    <t>IMM8</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>IMM6</t>
+  </si>
+  <si>
+    <t>IMM6s</t>
+  </si>
+  <si>
+    <t>IMM8s</t>
+  </si>
+  <si>
+    <t>IMM12</t>
+  </si>
+  <si>
+    <t>IMM12s</t>
   </si>
 </sst>
 </file>
@@ -1532,6 +1559,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1567,6 +1611,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1722,22 +1783,22 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="34.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="25.25" style="17" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" customWidth="1"/>
-    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.375" customWidth="1"/>
-    <col min="10" max="10" width="3.25" customWidth="1"/>
-    <col min="11" max="11" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="2" max="2" width="25.26953125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.36328125" customWidth="1"/>
+    <col min="5" max="5" width="5.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.36328125" customWidth="1"/>
+    <col min="10" max="10" width="3.26953125" customWidth="1"/>
+    <col min="11" max="11" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -1754,7 +1815,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="22" t="s">
         <v>60</v>
       </c>
@@ -1769,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>133</v>
       </c>
@@ -1784,7 +1845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -1799,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="30" t="s">
         <v>6</v>
       </c>
@@ -1814,7 +1875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="30" t="s">
         <v>9</v>
       </c>
@@ -1829,7 +1890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="30" t="s">
         <v>115</v>
       </c>
@@ -1844,7 +1905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
@@ -1859,7 +1920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="30" t="s">
         <v>17</v>
       </c>
@@ -1874,7 +1935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="30" t="s">
         <v>20</v>
       </c>
@@ -1889,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="30" t="s">
         <v>130</v>
       </c>
@@ -1904,7 +1965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="30" t="s">
         <v>25</v>
       </c>
@@ -1919,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="30" t="s">
         <v>9</v>
       </c>
@@ -1934,7 +1995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="30" t="s">
         <v>30</v>
       </c>
@@ -1949,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="30" t="s">
         <v>33</v>
       </c>
@@ -1964,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="30" t="s">
         <v>36</v>
       </c>
@@ -1979,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="30" t="s">
         <v>39</v>
       </c>
@@ -1994,7 +2055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="30" t="s">
         <v>97</v>
       </c>
@@ -2009,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="30" t="s">
         <v>100</v>
       </c>
@@ -2024,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="30" t="s">
         <v>136</v>
       </c>
@@ -2039,7 +2100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="30" t="s">
         <v>190</v>
       </c>
@@ -2054,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="30" t="s">
         <v>42</v>
       </c>
@@ -2069,7 +2130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
@@ -2084,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>73</v>
       </c>
@@ -2097,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25" s="26" t="s">
         <v>242</v>
@@ -2112,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
         <v>76</v>
       </c>
@@ -2127,7 +2188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
         <v>256</v>
@@ -2140,7 +2201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="30" t="s">
         <v>79</v>
       </c>
@@ -2155,7 +2216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="30" t="s">
         <v>82</v>
       </c>
@@ -2170,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="30" t="s">
         <v>137</v>
       </c>
@@ -2185,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="30" t="s">
         <v>138</v>
       </c>
@@ -2200,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="30" t="s">
         <v>107</v>
       </c>
@@ -2215,7 +2276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
         <v>197</v>
       </c>
@@ -2230,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="24"/>
       <c r="B34" s="26" t="s">
         <v>246</v>
@@ -2243,7 +2304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
         <v>65</v>
       </c>
@@ -2258,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
         <v>246</v>
@@ -2271,7 +2332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
         <v>198</v>
       </c>
@@ -2284,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
         <v>255</v>
@@ -2299,7 +2360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="22" t="s">
         <v>69</v>
       </c>
@@ -2312,7 +2373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="24"/>
       <c r="B40" s="26" t="s">
         <v>255</v>
@@ -2327,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="28" t="s">
         <v>85</v>
       </c>
@@ -2336,7 +2397,7 @@
       <c r="D41" s="20"/>
       <c r="E41" s="29"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="22" t="s">
         <v>201</v>
       </c>
@@ -2351,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="24"/>
       <c r="B43" s="26" t="s">
         <v>246</v>
@@ -2364,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="22" t="s">
         <v>87</v>
       </c>
@@ -2379,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
         <v>246</v>
@@ -2392,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="22" t="s">
         <v>91</v>
       </c>
@@ -2405,7 +2466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
         <v>260</v>
@@ -2420,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="22" t="s">
         <v>94</v>
       </c>
@@ -2435,7 +2496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
         <v>261</v>
@@ -2448,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="30" t="s">
         <v>51</v>
       </c>
@@ -2463,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="30" t="s">
         <v>48</v>
       </c>
@@ -2478,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="22" t="s">
         <v>54</v>
       </c>
@@ -2491,7 +2552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="28"/>
       <c r="B53" s="21" t="s">
         <v>259</v>
@@ -2502,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="24"/>
       <c r="B54" s="26" t="s">
         <v>257</v>
@@ -2515,7 +2576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="22" t="s">
         <v>152</v>
       </c>
@@ -2528,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="28"/>
       <c r="B56" s="21" t="s">
         <v>259</v>
@@ -2539,7 +2600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="24"/>
       <c r="B57" s="26" t="s">
         <v>258</v>
@@ -2552,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="22" t="s">
         <v>57</v>
       </c>
@@ -2567,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
         <v>262</v>
@@ -2580,7 +2641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="30" t="s">
         <v>155</v>
       </c>
@@ -2595,7 +2656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="30" t="s">
         <v>158</v>
       </c>
@@ -2610,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="30" t="s">
         <v>119</v>
       </c>
@@ -2625,7 +2686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="30" t="s">
         <v>122</v>
       </c>
@@ -2640,7 +2701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="30" t="s">
         <v>168</v>
       </c>
@@ -2655,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="30" t="s">
         <v>166</v>
       </c>
@@ -2670,7 +2731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="30" t="s">
         <v>163</v>
       </c>
@@ -2685,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="30" t="s">
         <v>124</v>
       </c>
@@ -2700,7 +2761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="30" t="s">
         <v>170</v>
       </c>
@@ -2715,7 +2776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="30" t="s">
         <v>174</v>
       </c>
@@ -2730,7 +2791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="30" t="s">
         <v>176</v>
       </c>
@@ -2745,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="30" t="s">
         <v>177</v>
       </c>
@@ -2760,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="30" t="s">
         <v>183</v>
       </c>
@@ -2775,7 +2836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="30" t="s">
         <v>182</v>
       </c>
@@ -2790,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="30" t="s">
         <v>202</v>
       </c>
@@ -2805,7 +2866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="30" t="s">
         <v>207</v>
       </c>
@@ -2820,7 +2881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="30" t="s">
         <v>215</v>
       </c>
@@ -2835,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="30" t="s">
         <v>212</v>
       </c>
@@ -2850,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="30" t="s">
         <v>188</v>
       </c>
@@ -2874,21 +2935,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="34.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
-    <col min="4" max="7" width="4.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="7" width="4.90625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.36328125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2909,7 +2970,7 @@
       </c>
       <c r="I1" s="37"/>
     </row>
-    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
@@ -2932,7 +2993,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>133</v>
       </c>
@@ -2961,7 +3022,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2984,7 +3045,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -3007,7 +3068,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3036,7 +3097,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>115</v>
       </c>
@@ -3065,7 +3126,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -3088,7 +3149,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -3111,7 +3172,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -3140,7 +3201,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>130</v>
       </c>
@@ -3169,7 +3230,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -3192,7 +3253,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -3221,7 +3282,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -3244,7 +3305,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -3273,7 +3334,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3296,7 +3357,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -3325,7 +3386,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>97</v>
       </c>
@@ -3348,7 +3409,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>100</v>
       </c>
@@ -3371,7 +3432,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>136</v>
       </c>
@@ -3400,7 +3461,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>190</v>
       </c>
@@ -3429,7 +3490,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -3446,7 +3507,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -3463,7 +3524,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -3480,7 +3541,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>76</v>
       </c>
@@ -3497,7 +3558,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>79</v>
       </c>
@@ -3514,7 +3575,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>82</v>
       </c>
@@ -3531,7 +3592,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>137</v>
       </c>
@@ -3548,7 +3609,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>138</v>
       </c>
@@ -3565,7 +3626,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>107</v>
       </c>
@@ -3582,7 +3643,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>197</v>
       </c>
@@ -3605,7 +3666,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -3634,7 +3695,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>198</v>
       </c>
@@ -3657,7 +3718,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
@@ -3686,7 +3747,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>85</v>
       </c>
@@ -3701,7 +3762,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>201</v>
       </c>
@@ -3724,7 +3785,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>87</v>
       </c>
@@ -3753,7 +3814,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>280</v>
       </c>
@@ -3770,7 +3831,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>279</v>
       </c>
@@ -3787,7 +3848,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
@@ -3810,7 +3871,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -3833,7 +3894,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>54</v>
       </c>
@@ -3856,7 +3917,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>152</v>
       </c>
@@ -3879,7 +3940,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -3896,7 +3957,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>155</v>
       </c>
@@ -3919,7 +3980,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>158</v>
       </c>
@@ -3942,7 +4003,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>119</v>
       </c>
@@ -3965,7 +4026,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>122</v>
       </c>
@@ -3988,7 +4049,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>168</v>
       </c>
@@ -4011,7 +4072,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>166</v>
       </c>
@@ -4034,7 +4095,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>163</v>
       </c>
@@ -4057,7 +4118,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>124</v>
       </c>
@@ -4080,7 +4141,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>170</v>
       </c>
@@ -4103,7 +4164,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>174</v>
       </c>
@@ -4126,7 +4187,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>176</v>
       </c>
@@ -4149,7 +4210,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>177</v>
       </c>
@@ -4172,7 +4233,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>183</v>
       </c>
@@ -4195,7 +4256,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>182</v>
       </c>
@@ -4218,7 +4279,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>202</v>
       </c>
@@ -4241,7 +4302,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>207</v>
       </c>
@@ -4270,7 +4331,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>215</v>
       </c>
@@ -4299,7 +4360,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>212</v>
       </c>
@@ -4328,7 +4389,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>188</v>
       </c>
@@ -4357,39 +4418,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
-    <col min="3" max="3" width="4.625" customWidth="1"/>
-    <col min="4" max="4" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.90625" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="4.6328125" customWidth="1"/>
+    <col min="4" max="4" width="7.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1" t="s">
         <v>296</v>
       </c>
-      <c r="B1" t="s">
-        <v>299</v>
-      </c>
-      <c r="C1" t="s">
-        <v>297</v>
-      </c>
       <c r="D1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E1" t="s">
         <v>294</v>
       </c>
-      <c r="E1" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -4406,7 +4473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>284</v>
       </c>
@@ -4414,7 +4481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>285</v>
       </c>
@@ -4422,7 +4489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>286</v>
       </c>
@@ -4430,7 +4497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>287</v>
       </c>
@@ -4438,7 +4505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>288</v>
       </c>
@@ -4446,7 +4513,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>289</v>
       </c>
@@ -4454,7 +4521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>290</v>
       </c>
@@ -4462,9 +4529,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B10" t="s">
         <v>292</v>
@@ -4479,7 +4546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>284</v>
       </c>
@@ -4487,7 +4554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>285</v>
       </c>
@@ -4495,7 +4562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>286</v>
       </c>
@@ -4503,7 +4570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>287</v>
       </c>
@@ -4511,7 +4578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>288</v>
       </c>
@@ -4519,7 +4586,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>289</v>
       </c>
@@ -4527,12 +4594,114 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>290</v>
       </c>
       <c r="E17">
         <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>304</v>
+      </c>
+      <c r="B18" t="s">
+        <v>300</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>305</v>
+      </c>
+      <c r="B19" t="s">
+        <v>300</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="F19">
+        <v>-31</v>
+      </c>
+      <c r="G19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" t="s">
+        <v>300</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>306</v>
+      </c>
+      <c r="B21" t="s">
+        <v>300</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="F21">
+        <v>-127</v>
+      </c>
+      <c r="G21">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>307</v>
+      </c>
+      <c r="B22" t="s">
+        <v>300</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" t="s">
+        <v>300</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <v>-2047</v>
+      </c>
+      <c r="G23">
+        <v>2048</v>
       </c>
     </row>
   </sheetData>
@@ -4548,14 +4717,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4566,7 +4735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -4577,7 +4746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
@@ -4588,7 +4757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -4599,7 +4768,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
@@ -4610,7 +4779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
         <v>115</v>
       </c>
@@ -4621,7 +4790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
         <v>207</v>
       </c>
@@ -4632,7 +4801,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
         <v>25</v>
       </c>
@@ -4643,7 +4812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
         <v>155</v>
       </c>
@@ -4654,7 +4823,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
         <v>158</v>
       </c>
@@ -4665,7 +4834,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
         <v>119</v>
       </c>
@@ -4676,7 +4845,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
         <v>122</v>
       </c>
@@ -4687,7 +4856,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
         <v>85</v>
       </c>
@@ -4696,7 +4865,7 @@
       </c>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
         <v>124</v>
       </c>
@@ -4707,7 +4876,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="11" t="s">
         <v>183</v>
       </c>
@@ -4718,7 +4887,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="11" t="s">
         <v>166</v>
       </c>
@@ -4729,7 +4898,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="11" t="s">
         <v>182</v>
       </c>
@@ -4740,7 +4909,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="11" t="s">
         <v>174</v>
       </c>
@@ -4751,7 +4920,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11" t="s">
         <v>163</v>
       </c>
@@ -4762,7 +4931,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11" t="s">
         <v>170</v>
       </c>
@@ -4773,7 +4942,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="11" t="s">
         <v>168</v>
       </c>
@@ -4784,7 +4953,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="11" t="s">
         <v>176</v>
       </c>
@@ -4795,7 +4964,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
         <v>177</v>
       </c>
@@ -4806,7 +4975,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="11" t="s">
         <v>54</v>
       </c>
@@ -4817,7 +4986,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="11" t="s">
         <v>100</v>
       </c>
@@ -4828,7 +4997,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="11" t="s">
         <v>136</v>
       </c>
@@ -4839,7 +5008,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="11" t="s">
         <v>190</v>
       </c>
@@ -4850,7 +5019,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="11" t="s">
         <v>97</v>
       </c>
@@ -4861,7 +5030,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="11" t="s">
         <v>42</v>
       </c>
@@ -4872,7 +5041,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="11" t="s">
         <v>138</v>
       </c>
@@ -4883,7 +5052,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="11" t="s">
         <v>36</v>
       </c>
@@ -4894,7 +5063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="11" t="s">
         <v>39</v>
       </c>
@@ -4905,7 +5074,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="11" t="s">
         <v>137</v>
       </c>
@@ -4916,7 +5085,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="11" t="s">
         <v>51</v>
       </c>
@@ -4927,7 +5096,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="11" t="s">
         <v>197</v>
       </c>
@@ -4938,7 +5107,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="11" t="s">
         <v>65</v>
       </c>
@@ -4949,7 +5118,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="11" t="s">
         <v>201</v>
       </c>
@@ -4960,7 +5129,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="11" t="s">
         <v>87</v>
       </c>
@@ -4971,7 +5140,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="11" t="s">
         <v>60</v>
       </c>
@@ -4982,7 +5151,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="11" t="s">
         <v>202</v>
       </c>
@@ -4993,7 +5162,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="11" t="s">
         <v>133</v>
       </c>
@@ -5004,7 +5173,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="11" t="s">
         <v>212</v>
       </c>
@@ -5015,7 +5184,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="11" t="s">
         <v>45</v>
       </c>
@@ -5026,7 +5195,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="11" t="s">
         <v>188</v>
       </c>
@@ -5037,7 +5206,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="11" t="s">
         <v>30</v>
       </c>
@@ -5048,7 +5217,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="11" t="s">
         <v>33</v>
       </c>
@@ -5059,7 +5228,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="11" t="s">
         <v>76</v>
       </c>
@@ -5070,7 +5239,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="11" t="s">
         <v>94</v>
       </c>
@@ -5081,7 +5250,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="11" t="s">
         <v>73</v>
       </c>
@@ -5092,7 +5261,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="11" t="s">
         <v>91</v>
       </c>
@@ -5103,7 +5272,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="11" t="s">
         <v>152</v>
       </c>
@@ -5114,7 +5283,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="11" t="s">
         <v>57</v>
       </c>
@@ -5125,7 +5294,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="11" t="s">
         <v>48</v>
       </c>
@@ -5136,7 +5305,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="11" t="s">
         <v>17</v>
       </c>
@@ -5147,7 +5316,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="11" t="s">
         <v>20</v>
       </c>
@@ -5158,7 +5327,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="11" t="s">
         <v>130</v>
       </c>
@@ -5169,7 +5338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="11" t="s">
         <v>130</v>
       </c>
@@ -5180,7 +5349,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="11" t="s">
         <v>79</v>
       </c>
@@ -5191,7 +5360,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="11" t="s">
         <v>82</v>
       </c>
@@ -5202,7 +5371,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="11" t="s">
         <v>198</v>
       </c>
@@ -5213,7 +5382,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="11" t="s">
         <v>69</v>
       </c>
@@ -5224,7 +5393,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="11" t="s">
         <v>14</v>
       </c>
@@ -5235,7 +5404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
operand parsed from aggregated operand parsers
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Documents\Programming\C#\Language\hasm\HasmParser\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joell\Documents\Programming\C#\Language\HomebrewAssembler\HasmParser\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="315">
   <si>
     <t>Instruction</t>
   </si>
@@ -985,6 +985,24 @@
   </si>
   <si>
     <t>IMM12s</t>
+  </si>
+  <si>
+    <t>PAIR</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>PAIR + IMM6s</t>
+  </si>
+  <si>
+    <t>LDD DST, PAIR + IMM6s</t>
   </si>
 </sst>
 </file>
@@ -1559,23 +1577,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1611,23 +1612,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1782,23 +1766,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="2" width="25.26953125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.36328125" customWidth="1"/>
-    <col min="5" max="5" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.36328125" customWidth="1"/>
-    <col min="10" max="10" width="3.26953125" customWidth="1"/>
-    <col min="11" max="11" width="8.453125" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="25.25" style="17" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" customWidth="1"/>
+    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.375" customWidth="1"/>
+    <col min="10" max="10" width="3.25" customWidth="1"/>
+    <col min="11" max="11" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -1815,7 +1799,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
         <v>60</v>
       </c>
@@ -1830,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
         <v>133</v>
       </c>
@@ -1845,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>3</v>
       </c>
@@ -1860,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>6</v>
       </c>
@@ -1875,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>9</v>
       </c>
@@ -1890,7 +1874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>115</v>
       </c>
@@ -1905,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
@@ -1920,7 +1904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>17</v>
       </c>
@@ -1935,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>20</v>
       </c>
@@ -1950,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>130</v>
       </c>
@@ -1965,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>25</v>
       </c>
@@ -1980,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>9</v>
       </c>
@@ -1995,7 +1979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>30</v>
       </c>
@@ -2010,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>33</v>
       </c>
@@ -2025,7 +2009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>36</v>
       </c>
@@ -2040,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>39</v>
       </c>
@@ -2055,7 +2039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>97</v>
       </c>
@@ -2070,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>100</v>
       </c>
@@ -2085,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>136</v>
       </c>
@@ -2100,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>190</v>
       </c>
@@ -2115,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>42</v>
       </c>
@@ -2130,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
@@ -2145,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>73</v>
       </c>
@@ -2158,7 +2142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="26" t="s">
         <v>242</v>
@@ -2173,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>76</v>
       </c>
@@ -2188,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
         <v>256</v>
@@ -2201,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>79</v>
       </c>
@@ -2216,7 +2200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="30" t="s">
         <v>82</v>
       </c>
@@ -2231,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="30" t="s">
         <v>137</v>
       </c>
@@ -2246,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
         <v>138</v>
       </c>
@@ -2261,7 +2245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="30" t="s">
         <v>107</v>
       </c>
@@ -2276,9 +2260,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>197</v>
+        <v>314</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>247</v>
@@ -2291,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
       <c r="B34" s="26" t="s">
         <v>246</v>
@@ -2304,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
         <v>65</v>
       </c>
@@ -2319,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
         <v>246</v>
@@ -2332,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>198</v>
       </c>
@@ -2345,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
         <v>255</v>
@@ -2360,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>69</v>
       </c>
@@ -2373,7 +2357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="26" t="s">
         <v>255</v>
@@ -2388,7 +2372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>85</v>
       </c>
@@ -2397,7 +2381,7 @@
       <c r="D41" s="20"/>
       <c r="E41" s="29"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>201</v>
       </c>
@@ -2412,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="26" t="s">
         <v>246</v>
@@ -2425,7 +2409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>87</v>
       </c>
@@ -2440,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
         <v>246</v>
@@ -2453,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>91</v>
       </c>
@@ -2466,7 +2450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
         <v>260</v>
@@ -2481,7 +2465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>94</v>
       </c>
@@ -2496,7 +2480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
         <v>261</v>
@@ -2509,7 +2493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>51</v>
       </c>
@@ -2524,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="30" t="s">
         <v>48</v>
       </c>
@@ -2539,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>54</v>
       </c>
@@ -2552,7 +2536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
       <c r="B53" s="21" t="s">
         <v>259</v>
@@ -2563,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="26" t="s">
         <v>257</v>
@@ -2576,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>152</v>
       </c>
@@ -2589,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="28"/>
       <c r="B56" s="21" t="s">
         <v>259</v>
@@ -2600,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="26" t="s">
         <v>258</v>
@@ -2613,7 +2597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
         <v>57</v>
       </c>
@@ -2628,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
         <v>262</v>
@@ -2641,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="30" t="s">
         <v>155</v>
       </c>
@@ -2656,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="30" t="s">
         <v>158</v>
       </c>
@@ -2671,7 +2655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>119</v>
       </c>
@@ -2686,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
         <v>122</v>
       </c>
@@ -2701,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="30" t="s">
         <v>168</v>
       </c>
@@ -2716,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="30" t="s">
         <v>166</v>
       </c>
@@ -2731,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="30" t="s">
         <v>163</v>
       </c>
@@ -2746,7 +2730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="30" t="s">
         <v>124</v>
       </c>
@@ -2761,7 +2745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="30" t="s">
         <v>170</v>
       </c>
@@ -2776,7 +2760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="30" t="s">
         <v>174</v>
       </c>
@@ -2791,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>176</v>
       </c>
@@ -2806,7 +2790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="30" t="s">
         <v>177</v>
       </c>
@@ -2821,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="30" t="s">
         <v>183</v>
       </c>
@@ -2836,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>182</v>
       </c>
@@ -2851,7 +2835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
         <v>202</v>
       </c>
@@ -2866,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>207</v>
       </c>
@@ -2881,7 +2865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
         <v>215</v>
       </c>
@@ -2896,7 +2880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
         <v>212</v>
       </c>
@@ -2911,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="30" t="s">
         <v>188</v>
       </c>
@@ -2935,21 +2919,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
-    <col min="4" max="7" width="4.90625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="4" max="7" width="4.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2970,7 +2954,7 @@
       </c>
       <c r="I1" s="37"/>
     </row>
-    <row r="2" spans="1:9" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>60</v>
       </c>
@@ -2993,7 +2977,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>133</v>
       </c>
@@ -3022,7 +3006,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3045,7 +3029,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -3068,7 +3052,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3097,7 +3081,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>115</v>
       </c>
@@ -3126,7 +3110,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -3149,7 +3133,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -3172,7 +3156,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -3201,7 +3185,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>130</v>
       </c>
@@ -3230,7 +3214,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>25</v>
       </c>
@@ -3253,7 +3237,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -3282,7 +3266,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -3305,7 +3289,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>33</v>
       </c>
@@ -3334,7 +3318,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -3357,7 +3341,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -3386,7 +3370,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>97</v>
       </c>
@@ -3409,7 +3393,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>100</v>
       </c>
@@ -3432,7 +3416,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>136</v>
       </c>
@@ -3461,7 +3445,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>190</v>
       </c>
@@ -3490,7 +3474,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -3507,7 +3491,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -3524,7 +3508,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -3541,7 +3525,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>76</v>
       </c>
@@ -3558,7 +3542,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>79</v>
       </c>
@@ -3575,7 +3559,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>82</v>
       </c>
@@ -3592,7 +3576,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>137</v>
       </c>
@@ -3609,7 +3593,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>138</v>
       </c>
@@ -3626,7 +3610,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>107</v>
       </c>
@@ -3643,9 +3627,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>197</v>
+        <v>314</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>68</v>
@@ -3666,7 +3650,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -3695,7 +3679,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>198</v>
       </c>
@@ -3718,7 +3702,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>69</v>
       </c>
@@ -3747,7 +3731,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>85</v>
       </c>
@@ -3762,7 +3746,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>201</v>
       </c>
@@ -3785,7 +3769,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>87</v>
       </c>
@@ -3814,7 +3798,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>280</v>
       </c>
@@ -3831,7 +3815,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>279</v>
       </c>
@@ -3848,7 +3832,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
@@ -3871,7 +3855,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -3894,7 +3878,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>54</v>
       </c>
@@ -3917,7 +3901,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>152</v>
       </c>
@@ -3940,7 +3924,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
@@ -3957,7 +3941,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>155</v>
       </c>
@@ -3980,7 +3964,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>158</v>
       </c>
@@ -4003,7 +3987,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>119</v>
       </c>
@@ -4026,7 +4010,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>122</v>
       </c>
@@ -4049,7 +4033,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>168</v>
       </c>
@@ -4072,7 +4056,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>166</v>
       </c>
@@ -4095,7 +4079,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>163</v>
       </c>
@@ -4118,7 +4102,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>124</v>
       </c>
@@ -4141,7 +4125,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>170</v>
       </c>
@@ -4164,7 +4148,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>174</v>
       </c>
@@ -4187,7 +4171,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>176</v>
       </c>
@@ -4210,7 +4194,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>177</v>
       </c>
@@ -4233,7 +4217,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>183</v>
       </c>
@@ -4256,7 +4240,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>182</v>
       </c>
@@ -4279,7 +4263,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>202</v>
       </c>
@@ -4302,7 +4286,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>207</v>
       </c>
@@ -4331,7 +4315,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>215</v>
       </c>
@@ -4360,7 +4344,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>212</v>
       </c>
@@ -4389,7 +4373,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>188</v>
       </c>
@@ -4418,22 +4402,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.90625" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" customWidth="1"/>
-    <col min="3" max="3" width="4.6328125" customWidth="1"/>
-    <col min="4" max="4" width="7.26953125" customWidth="1"/>
-    <col min="5" max="5" width="6.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.875" customWidth="1"/>
+    <col min="2" max="2" width="13.25" customWidth="1"/>
+    <col min="3" max="3" width="4.625" customWidth="1"/>
+    <col min="4" max="4" width="7.25" customWidth="1"/>
+    <col min="5" max="5" width="6.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>295</v>
       </c>
@@ -4456,7 +4440,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -4473,7 +4457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>284</v>
       </c>
@@ -4481,7 +4465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>285</v>
       </c>
@@ -4489,7 +4473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>286</v>
       </c>
@@ -4497,7 +4481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>287</v>
       </c>
@@ -4505,7 +4489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>288</v>
       </c>
@@ -4513,7 +4497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>289</v>
       </c>
@@ -4521,7 +4505,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>290</v>
       </c>
@@ -4529,7 +4513,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>297</v>
       </c>
@@ -4546,7 +4530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>284</v>
       </c>
@@ -4554,7 +4538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>285</v>
       </c>
@@ -4562,7 +4546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>286</v>
       </c>
@@ -4570,7 +4554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>287</v>
       </c>
@@ -4578,7 +4562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>288</v>
       </c>
@@ -4586,7 +4570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>289</v>
       </c>
@@ -4594,7 +4578,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>290</v>
       </c>
@@ -4602,7 +4586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>304</v>
       </c>
@@ -4619,7 +4603,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>305</v>
       </c>
@@ -4636,7 +4620,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>299</v>
       </c>
@@ -4653,7 +4637,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>306</v>
       </c>
@@ -4670,7 +4654,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>307</v>
       </c>
@@ -4687,7 +4671,7 @@
         <v>4096</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>308</v>
       </c>
@@ -4702,6 +4686,36 @@
       </c>
       <c r="G23">
         <v>2048</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>309</v>
+      </c>
+      <c r="B24" t="s">
+        <v>310</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24" t="s">
+        <v>311</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>312</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -4717,14 +4731,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -4735,7 +4749,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>6</v>
       </c>
@@ -4746,7 +4760,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>3</v>
       </c>
@@ -4757,7 +4771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -4768,7 +4782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>9</v>
       </c>
@@ -4779,7 +4793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>115</v>
       </c>
@@ -4790,7 +4804,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>207</v>
       </c>
@@ -4801,7 +4815,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>25</v>
       </c>
@@ -4812,7 +4826,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>155</v>
       </c>
@@ -4823,7 +4837,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>158</v>
       </c>
@@ -4834,7 +4848,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>119</v>
       </c>
@@ -4845,7 +4859,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>122</v>
       </c>
@@ -4856,7 +4870,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>85</v>
       </c>
@@ -4865,7 +4879,7 @@
       </c>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>124</v>
       </c>
@@ -4876,7 +4890,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>183</v>
       </c>
@@ -4887,7 +4901,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>166</v>
       </c>
@@ -4898,7 +4912,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>182</v>
       </c>
@@ -4909,7 +4923,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>174</v>
       </c>
@@ -4920,7 +4934,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>163</v>
       </c>
@@ -4931,7 +4945,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>170</v>
       </c>
@@ -4942,7 +4956,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>168</v>
       </c>
@@ -4953,7 +4967,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>176</v>
       </c>
@@ -4964,7 +4978,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>177</v>
       </c>
@@ -4975,7 +4989,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>54</v>
       </c>
@@ -4986,7 +5000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>100</v>
       </c>
@@ -4997,7 +5011,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>136</v>
       </c>
@@ -5008,7 +5022,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>190</v>
       </c>
@@ -5019,7 +5033,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>97</v>
       </c>
@@ -5030,7 +5044,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>42</v>
       </c>
@@ -5041,7 +5055,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>138</v>
       </c>
@@ -5052,7 +5066,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>36</v>
       </c>
@@ -5063,7 +5077,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>39</v>
       </c>
@@ -5074,7 +5088,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>137</v>
       </c>
@@ -5085,7 +5099,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>51</v>
       </c>
@@ -5096,7 +5110,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>197</v>
       </c>
@@ -5107,7 +5121,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>65</v>
       </c>
@@ -5118,7 +5132,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>201</v>
       </c>
@@ -5129,7 +5143,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>87</v>
       </c>
@@ -5140,7 +5154,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>60</v>
       </c>
@@ -5151,7 +5165,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>202</v>
       </c>
@@ -5162,7 +5176,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>133</v>
       </c>
@@ -5173,7 +5187,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>212</v>
       </c>
@@ -5184,7 +5198,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>45</v>
       </c>
@@ -5195,7 +5209,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>188</v>
       </c>
@@ -5206,7 +5220,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>30</v>
       </c>
@@ -5217,7 +5231,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>33</v>
       </c>
@@ -5228,7 +5242,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>76</v>
       </c>
@@ -5239,7 +5253,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>94</v>
       </c>
@@ -5250,7 +5264,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>73</v>
       </c>
@@ -5261,7 +5275,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>91</v>
       </c>
@@ -5272,7 +5286,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
         <v>152</v>
       </c>
@@ -5283,7 +5297,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
         <v>57</v>
       </c>
@@ -5294,7 +5308,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
         <v>48</v>
       </c>
@@ -5305,7 +5319,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>17</v>
       </c>
@@ -5316,7 +5330,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>20</v>
       </c>
@@ -5327,7 +5341,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>130</v>
       </c>
@@ -5338,7 +5352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>130</v>
       </c>
@@ -5349,7 +5363,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
         <v>79</v>
       </c>
@@ -5360,7 +5374,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
         <v>82</v>
       </c>
@@ -5371,7 +5385,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
         <v>198</v>
       </c>
@@ -5382,7 +5396,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>69</v>
       </c>
@@ -5393,7 +5407,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
         <v>14</v>
       </c>
@@ -5404,7 +5418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
added the special purpose register operands
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="323">
   <si>
     <t>Instruction</t>
   </si>
@@ -642,12 +642,6 @@
     <t>DST &lt;- PROG[PAIR + IMM6]</t>
   </si>
   <si>
-    <t>1sss</t>
-  </si>
-  <si>
-    <t>0sss</t>
-  </si>
-  <si>
     <t>dpkk</t>
   </si>
   <si>
@@ -1003,6 +997,36 @@
   </si>
   <si>
     <t>LDD DST, PAIR + IMM6s</t>
+  </si>
+  <si>
+    <t>SPC,SPC1</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>MAR</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>MDR</t>
+  </si>
+  <si>
+    <t>SREG</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>SPC2</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>0DDD</t>
   </si>
 </sst>
 </file>
@@ -1787,16 +1811,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1804,11 +1828,11 @@
         <v>60</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E2" s="23">
         <v>1</v>
@@ -1819,11 +1843,11 @@
         <v>133</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E3" s="23">
         <v>1</v>
@@ -1834,11 +1858,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E4" s="33">
         <v>1</v>
@@ -1849,11 +1873,11 @@
         <v>6</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E5" s="33">
         <v>1</v>
@@ -1864,11 +1888,11 @@
         <v>9</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E6" s="33">
         <v>1</v>
@@ -1879,11 +1903,11 @@
         <v>115</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E7" s="33">
         <v>1</v>
@@ -1894,11 +1918,11 @@
         <v>14</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E8" s="33">
         <v>1</v>
@@ -1909,11 +1933,11 @@
         <v>17</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E9" s="33">
         <v>1</v>
@@ -1924,11 +1948,11 @@
         <v>20</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E10" s="33">
         <v>1</v>
@@ -1939,11 +1963,11 @@
         <v>130</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E11" s="33">
         <v>1</v>
@@ -1954,11 +1978,11 @@
         <v>25</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E12" s="33">
         <v>1</v>
@@ -1969,11 +1993,11 @@
         <v>9</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E13" s="33">
         <v>1</v>
@@ -1984,11 +2008,11 @@
         <v>30</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E14" s="33">
         <v>1</v>
@@ -1999,11 +2023,11 @@
         <v>33</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E15" s="33">
         <v>1</v>
@@ -2014,11 +2038,11 @@
         <v>36</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E16" s="33">
         <v>1</v>
@@ -2029,11 +2053,11 @@
         <v>39</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E17" s="33">
         <v>1</v>
@@ -2044,11 +2068,11 @@
         <v>97</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E18" s="33">
         <v>1</v>
@@ -2059,11 +2083,11 @@
         <v>100</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E19" s="33">
         <v>1</v>
@@ -2074,11 +2098,11 @@
         <v>136</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E20" s="33">
         <v>1</v>
@@ -2089,11 +2113,11 @@
         <v>190</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E21" s="33">
         <v>1</v>
@@ -2104,11 +2128,11 @@
         <v>42</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E22" s="33">
         <v>1</v>
@@ -2119,11 +2143,11 @@
         <v>45</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E23" s="23">
         <v>1</v>
@@ -2134,7 +2158,7 @@
         <v>73</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -2145,13 +2169,13 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>244</v>
-      </c>
       <c r="D25" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E25" s="27">
         <v>0</v>
@@ -2162,10 +2186,10 @@
         <v>76</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="23">
@@ -2175,11 +2199,11 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E27" s="27">
         <v>0</v>
@@ -2190,11 +2214,11 @@
         <v>79</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E28" s="33">
         <v>1</v>
@@ -2205,11 +2229,11 @@
         <v>82</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E29" s="33">
         <v>1</v>
@@ -2220,11 +2244,11 @@
         <v>137</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E30" s="33">
         <v>1</v>
@@ -2235,11 +2259,11 @@
         <v>138</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E31" s="33">
         <v>1</v>
@@ -2250,11 +2274,11 @@
         <v>107</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E32" s="33">
         <v>1</v>
@@ -2262,13 +2286,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="23">
@@ -2278,11 +2302,11 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="24"/>
       <c r="B34" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E34" s="27">
         <v>0</v>
@@ -2293,10 +2317,10 @@
         <v>65</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="23">
@@ -2306,11 +2330,11 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="24"/>
       <c r="B36" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E36" s="27">
         <v>0</v>
@@ -2318,10 +2342,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -2332,13 +2356,13 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="24"/>
       <c r="B38" s="26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E38" s="27">
         <v>0</v>
@@ -2349,7 +2373,7 @@
         <v>69</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -2360,13 +2384,13 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="24"/>
       <c r="B40" s="26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E40" s="27">
         <v>0</v>
@@ -2383,13 +2407,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="23">
@@ -2399,11 +2423,11 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="24"/>
       <c r="B43" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E43" s="27">
         <v>0</v>
@@ -2414,10 +2438,10 @@
         <v>87</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="23">
@@ -2427,11 +2451,11 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="24"/>
       <c r="B45" s="26" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E45" s="27">
         <v>0</v>
@@ -2442,7 +2466,7 @@
         <v>91</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -2453,13 +2477,13 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
       <c r="B47" s="26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E47" s="27">
         <v>0</v>
@@ -2470,10 +2494,10 @@
         <v>94</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D48" s="18"/>
       <c r="E48" s="23">
@@ -2483,11 +2507,11 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="24"/>
       <c r="B49" s="26" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C49" s="25"/>
       <c r="D49" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E49" s="27">
         <v>0</v>
@@ -2498,11 +2522,11 @@
         <v>51</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E50" s="33">
         <v>0</v>
@@ -2513,11 +2537,11 @@
         <v>48</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E51" s="33">
         <v>0</v>
@@ -2528,7 +2552,7 @@
         <v>54</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -2539,7 +2563,7 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="28"/>
       <c r="B53" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
@@ -2550,11 +2574,11 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="24"/>
       <c r="B54" s="26" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E54" s="27">
         <v>0</v>
@@ -2565,7 +2589,7 @@
         <v>152</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2576,7 +2600,7 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="28"/>
       <c r="B56" s="21" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -2587,11 +2611,11 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="24"/>
       <c r="B57" s="26" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E57" s="27">
         <v>0</v>
@@ -2602,10 +2626,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="23">
@@ -2615,11 +2639,11 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="24"/>
       <c r="B59" s="26" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E59" s="27">
         <v>0</v>
@@ -2630,11 +2654,11 @@
         <v>155</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E60" s="33">
         <v>0</v>
@@ -2645,11 +2669,11 @@
         <v>158</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E61" s="33">
         <v>0</v>
@@ -2660,11 +2684,11 @@
         <v>119</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E62" s="33">
         <v>0</v>
@@ -2675,11 +2699,11 @@
         <v>122</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E63" s="33">
         <v>0</v>
@@ -2690,11 +2714,11 @@
         <v>168</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E64" s="33">
         <v>0</v>
@@ -2705,11 +2729,11 @@
         <v>166</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E65" s="33">
         <v>0</v>
@@ -2720,11 +2744,11 @@
         <v>163</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E66" s="33">
         <v>0</v>
@@ -2735,11 +2759,11 @@
         <v>124</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E67" s="33">
         <v>0</v>
@@ -2750,11 +2774,11 @@
         <v>170</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E68" s="33">
         <v>0</v>
@@ -2765,11 +2789,11 @@
         <v>174</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C69" s="31"/>
       <c r="D69" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E69" s="33">
         <v>0</v>
@@ -2780,11 +2804,11 @@
         <v>176</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E70" s="33">
         <v>0</v>
@@ -2795,11 +2819,11 @@
         <v>177</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E71" s="33">
         <v>0</v>
@@ -2810,11 +2834,11 @@
         <v>183</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E72" s="33">
         <v>0</v>
@@ -2825,11 +2849,11 @@
         <v>182</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E73" s="33">
         <v>0</v>
@@ -2837,14 +2861,14 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C74" s="31"/>
       <c r="D74" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E74" s="33">
         <v>0</v>
@@ -2852,14 +2876,14 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E75" s="33">
         <v>0</v>
@@ -2867,14 +2891,14 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E76" s="33">
         <v>0</v>
@@ -2882,14 +2906,14 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C77" s="31"/>
       <c r="D77" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E77" s="33">
         <v>0</v>
@@ -2904,7 +2928,7 @@
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E78" s="33">
         <v>0</v>
@@ -2919,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3629,7 +3653,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>68</v>
@@ -3644,7 +3668,7 @@
         <v>147</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>114</v>
@@ -3681,7 +3705,7 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>72</v>
@@ -3693,10 +3717,10 @@
         <v>116</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>114</v>
@@ -3748,7 +3772,7 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>90</v>
@@ -3763,7 +3787,7 @@
         <v>148</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>114</v>
@@ -3800,36 +3824,36 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>150</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>195</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>95</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>150</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4265,13 +4289,13 @@
     </row>
     <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>204</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>112</v>
@@ -4280,21 +4304,21 @@
         <v>135</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>209</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>151</v>
@@ -4303,7 +4327,7 @@
         <v>113</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G60" s="8" t="s">
         <v>114</v>
@@ -4317,13 +4341,13 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>151</v>
@@ -4332,7 +4356,7 @@
         <v>116</v>
       </c>
       <c r="F61" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G61" s="8" t="s">
         <v>114</v>
@@ -4346,13 +4370,13 @@
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>214</v>
       </c>
       <c r="D62" s="8" t="s">
         <v>151</v>
@@ -4361,7 +4385,7 @@
         <v>112</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G62" s="8" t="s">
         <v>114</v>
@@ -4402,10 +4426,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:G26"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4419,39 +4443,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G1" t="s">
         <v>301</v>
-      </c>
-      <c r="E1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F1" t="s">
-        <v>302</v>
-      </c>
-      <c r="G1" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -4459,7 +4483,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -4467,7 +4491,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -4475,7 +4499,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -4483,7 +4507,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -4491,7 +4515,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -4499,7 +4523,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -4507,7 +4531,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -4515,16 +4539,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -4532,7 +4556,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -4540,7 +4564,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -4548,7 +4572,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -4556,7 +4580,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -4564,7 +4588,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E15">
         <v>5</v>
@@ -4572,7 +4596,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -4580,7 +4604,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E17">
         <v>7</v>
@@ -4588,10 +4612,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -4605,10 +4629,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B19" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C19">
         <v>6</v>
@@ -4622,10 +4646,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B20" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C20">
         <v>8</v>
@@ -4639,10 +4663,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C21">
         <v>8</v>
@@ -4656,10 +4680,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B22" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C22">
         <v>12</v>
@@ -4673,10 +4697,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B23" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C23">
         <v>12</v>
@@ -4690,16 +4714,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -4707,7 +4731,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -4716,6 +4740,136 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>313</v>
+      </c>
+      <c r="B26" t="s">
+        <v>314</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>316</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>317</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>315</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>318</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>309</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>310</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>319</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B33" t="s">
+        <v>321</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>316</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>317</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>315</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>318</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>309</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>310</v>
+      </c>
+      <c r="E38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>319</v>
+      </c>
+      <c r="E39">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -4806,13 +4960,13 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>207</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5112,7 +5266,7 @@
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>68</v>
@@ -5134,7 +5288,7 @@
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>90</v>
@@ -5167,13 +5321,13 @@
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>202</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5189,13 +5343,13 @@
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>212</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5357,10 +5511,10 @@
         <v>130</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5387,7 +5541,7 @@
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
uhasm is able to tokenize all alu operations
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
   </bookViews>
   <sheets>
     <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
@@ -605,9 +605,6 @@
     <t>DST - IMM8 - C</t>
   </si>
   <si>
-    <t xml:space="preserve">0xFF – DST </t>
-  </si>
-  <si>
     <t>0x00 - DST</t>
   </si>
   <si>
@@ -953,40 +950,43 @@
     <t>PC = PC + IMM8s</t>
   </si>
   <si>
-    <t>if ccc = 0 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if ccc = 1 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if C = 0 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if C = 1 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if Z = 0 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if Z = 1 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if N = 0 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if N = 1 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if V = 0 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if V = 1 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if S = 0 PC = PC + IMM8s</t>
-  </si>
-  <si>
-    <t>if S = 1 PC = PC + IMM8s</t>
+    <t>if ccc = 0: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if C = 0: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if Z = 0: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if N = 0: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if V = 0: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if S = 0: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if ccc = 1: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if C = 1: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if Z = 1: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if N = 1: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if V = 1: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t>if S = 1: PC = PC + IMM8s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0xFF - DST </t>
   </si>
 </sst>
 </file>
@@ -1377,15 +1377,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1404,29 +1395,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1502,13 +1484,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thick">
-          <color rgb="FFC9C9C9"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="medium">
           <color rgb="FFDBDBDB"/>
         </left>
@@ -1519,6 +1494,31 @@
           <color rgb="FFDBDBDB"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thick">
+          <color rgb="FFC9C9C9"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1534,12 +1534,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:C63" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:C63" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:C63"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Instruction" dataDxfId="3"/>
-    <tableColumn id="2" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" name="Semantic" dataDxfId="1"/>
+    <tableColumn id="1" name="Instruction" dataDxfId="2"/>
+    <tableColumn id="2" name="Description" dataDxfId="1"/>
+    <tableColumn id="3" name="Semantic" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1810,20 +1810,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="26.875" style="17" customWidth="1"/>
-    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.375" customWidth="1"/>
-    <col min="5" max="5" width="5.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.375" customWidth="1"/>
-    <col min="10" max="10" width="3.25" customWidth="1"/>
-    <col min="11" max="11" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" style="17" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1831,20 +1831,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>200</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>196</v>
-      </c>
       <c r="E1" s="36" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="37" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -1852,14 +1852,14 @@
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E2" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="37" t="s">
         <v>119</v>
       </c>
       <c r="B3" s="19" t="s">
@@ -1867,14 +1867,14 @@
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E3" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="32" t="s">
@@ -1882,14 +1882,14 @@
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E4" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="32" t="s">
@@ -1897,14 +1897,14 @@
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E5" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -1912,14 +1912,14 @@
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E6" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="38" t="s">
         <v>107</v>
       </c>
       <c r="B7" s="32" t="s">
@@ -1927,14 +1927,14 @@
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E7" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="38" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="32" t="s">
@@ -1942,14 +1942,14 @@
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E8" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="32" t="s">
@@ -1957,14 +1957,14 @@
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E9" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="38" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="32" t="s">
@@ -1972,14 +1972,14 @@
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E10" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="38" t="s">
         <v>116</v>
       </c>
       <c r="B11" s="32" t="s">
@@ -1987,14 +1987,14 @@
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E11" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="38" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="32" t="s">
@@ -2002,14 +2002,14 @@
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E12" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="32" t="s">
@@ -2017,14 +2017,14 @@
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E13" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="38" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="32" t="s">
@@ -2032,14 +2032,14 @@
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E14" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="38" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="32" t="s">
@@ -2047,14 +2047,14 @@
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E15" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="38" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="32" t="s">
@@ -2062,14 +2062,14 @@
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E16" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="38" t="s">
         <v>37</v>
       </c>
       <c r="B17" s="32" t="s">
@@ -2077,14 +2077,14 @@
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E17" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="38" t="s">
         <v>90</v>
       </c>
       <c r="B18" s="32" t="s">
@@ -2092,14 +2092,14 @@
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E18" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="38" t="s">
         <v>93</v>
       </c>
       <c r="B19" s="32" t="s">
@@ -2107,14 +2107,14 @@
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E19" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+      <c r="A20" s="38" t="s">
         <v>122</v>
       </c>
       <c r="B20" s="32" t="s">
@@ -2122,14 +2122,14 @@
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E20" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
+      <c r="A21" s="38" t="s">
         <v>155</v>
       </c>
       <c r="B21" s="32" t="s">
@@ -2137,48 +2137,48 @@
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E21" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="38" t="s">
         <v>40</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>192</v>
+        <v>319</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E22" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E23" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="37" t="s">
         <v>68</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -2187,29 +2187,29 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="42"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C25" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>201</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>202</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="23">
@@ -2217,102 +2217,102 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E27" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="38" t="s">
         <v>74</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="38" t="s">
         <v>77</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E29" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="38" t="s">
         <v>123</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E30" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="38" t="s">
         <v>124</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E31" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="38" t="s">
         <v>99</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E32" s="33">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="40" t="s">
-        <v>257</v>
+      <c r="A33" s="37" t="s">
+        <v>256</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="23">
@@ -2320,27 +2320,27 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="42"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E34" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="37" t="s">
         <v>60</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="23">
@@ -2348,24 +2348,24 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E36" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
-        <v>299</v>
+      <c r="A37" s="37" t="s">
+        <v>298</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -2374,26 +2374,26 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
+      <c r="A38" s="39"/>
       <c r="B38" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E38" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="37" t="s">
         <v>64</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -2402,22 +2402,22 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="39"/>
       <c r="B40" s="26" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E40" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
+      <c r="A41" s="40" t="s">
         <v>80</v>
       </c>
       <c r="B41" s="21"/>
@@ -2426,14 +2426,14 @@
       <c r="E41" s="29"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
-        <v>301</v>
+      <c r="A42" s="37" t="s">
+        <v>300</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="23">
@@ -2441,27 +2441,27 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="39"/>
       <c r="B43" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E43" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
+      <c r="A44" s="37" t="s">
         <v>82</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="23">
@@ -2469,24 +2469,24 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E45" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="37" t="s">
         <v>86</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -2495,29 +2495,29 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
+      <c r="A47" s="39"/>
       <c r="B47" s="26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C47" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="E47" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C48" s="18" t="s">
         <v>201</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E47" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>202</v>
       </c>
       <c r="D48" s="18"/>
       <c r="E48" s="23">
@@ -2525,54 +2525,54 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="42"/>
+      <c r="A49" s="39"/>
       <c r="B49" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C49" s="25"/>
       <c r="D49" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E49" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="41" t="s">
+      <c r="A50" s="38" t="s">
         <v>47</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E50" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="41" t="s">
-        <v>268</v>
+      <c r="A51" s="38" t="s">
+        <v>267</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E51" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="40" t="s">
+      <c r="A52" s="37" t="s">
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -2581,9 +2581,9 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="43"/>
+      <c r="A53" s="40"/>
       <c r="B53" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
@@ -2592,24 +2592,24 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="42"/>
+      <c r="A54" s="39"/>
       <c r="B54" s="26" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E54" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="40" t="s">
-        <v>271</v>
+      <c r="A55" s="37" t="s">
+        <v>270</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2618,9 +2618,9 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="43"/>
+      <c r="A56" s="40"/>
       <c r="B56" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C56" s="20"/>
       <c r="D56" s="20"/>
@@ -2629,27 +2629,27 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="42"/>
+      <c r="A57" s="39"/>
       <c r="B57" s="26" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E57" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="40" t="s">
+      <c r="A58" s="37" t="s">
         <v>52</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="23">
@@ -2657,290 +2657,290 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="42"/>
+      <c r="A59" s="39"/>
       <c r="B59" s="26" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="25" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E59" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="41" t="s">
-        <v>272</v>
+      <c r="A60" s="38" t="s">
+        <v>271</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E60" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="41" t="s">
-        <v>274</v>
+      <c r="A61" s="38" t="s">
+        <v>273</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E61" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="41" t="s">
-        <v>276</v>
+      <c r="A62" s="38" t="s">
+        <v>275</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E62" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="41" t="s">
-        <v>278</v>
+      <c r="A63" s="38" t="s">
+        <v>277</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E63" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="41" t="s">
-        <v>280</v>
+      <c r="A64" s="38" t="s">
+        <v>279</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E64" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="41" t="s">
-        <v>281</v>
+      <c r="A65" s="38" t="s">
+        <v>280</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E65" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="41" t="s">
-        <v>282</v>
+      <c r="A66" s="38" t="s">
+        <v>281</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E66" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="41" t="s">
-        <v>284</v>
+      <c r="A67" s="38" t="s">
+        <v>283</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E67" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="41" t="s">
-        <v>286</v>
+      <c r="A68" s="38" t="s">
+        <v>285</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E68" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="41" t="s">
-        <v>288</v>
+      <c r="A69" s="38" t="s">
+        <v>287</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C69" s="31"/>
       <c r="D69" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E69" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="41" t="s">
-        <v>290</v>
+      <c r="A70" s="38" t="s">
+        <v>289</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E70" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="41" t="s">
-        <v>292</v>
+      <c r="A71" s="38" t="s">
+        <v>291</v>
       </c>
       <c r="B71" s="32" t="s">
         <v>317</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E71" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="41" t="s">
-        <v>294</v>
+      <c r="A72" s="38" t="s">
+        <v>293</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E72" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="41" t="s">
-        <v>296</v>
+      <c r="A73" s="38" t="s">
+        <v>295</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E73" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="41" t="s">
+      <c r="A74" s="38" t="s">
         <v>159</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C74" s="31"/>
       <c r="D74" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E74" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="41" t="s">
+      <c r="A75" s="38" t="s">
         <v>164</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E75" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="41" t="s">
+      <c r="A76" s="38" t="s">
         <v>172</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E76" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="41" t="s">
+      <c r="A77" s="38" t="s">
         <v>169</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C77" s="31"/>
       <c r="D77" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E77" s="33">
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="41" t="s">
+      <c r="A78" s="38" t="s">
         <v>153</v>
       </c>
       <c r="B78" s="32" t="s">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E78" s="33">
         <v>0</v>
@@ -2968,14 +2968,14 @@
       <selection sqref="A1:C63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
-    <col min="4" max="7" width="4.875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="7" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2988,16 +2988,16 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39" t="s">
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="57" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="37"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -3131,7 +3131,7 @@
         <v>107</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
@@ -3235,7 +3235,7 @@
         <v>116</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>22</v>
@@ -3495,7 +3495,7 @@
         <v>155</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>98</v>
@@ -3674,13 +3674,13 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>108</v>
@@ -3726,13 +3726,13 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>108</v>
@@ -3793,13 +3793,13 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>108</v>
@@ -3845,30 +3845,30 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>136</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>136</v>
@@ -3902,13 +3902,13 @@
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>105</v>
@@ -3931,7 +3931,7 @@
         <v>51</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>118</v>
@@ -3948,13 +3948,13 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>138</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>105</v>
@@ -3988,13 +3988,13 @@
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>111</v>
@@ -4011,13 +4011,13 @@
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>141</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>111</v>
@@ -4034,13 +4034,13 @@
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>111</v>
@@ -4057,13 +4057,13 @@
     </row>
     <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>111</v>
@@ -4080,13 +4080,13 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>146</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>111</v>
@@ -4103,13 +4103,13 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>145</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>111</v>
@@ -4126,13 +4126,13 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>144</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>111</v>
@@ -4149,13 +4149,13 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>111</v>
@@ -4172,13 +4172,13 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>147</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>111</v>
@@ -4195,13 +4195,13 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>111</v>
@@ -4218,13 +4218,13 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>149</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>111</v>
@@ -4241,13 +4241,13 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>111</v>
@@ -4264,13 +4264,13 @@
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>151</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>111</v>
@@ -4287,13 +4287,13 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>152</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>111</v>
@@ -4360,7 +4360,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>172</v>
       </c>
@@ -4455,604 +4455,604 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.875" customWidth="1"/>
-    <col min="2" max="2" width="13.25" customWidth="1"/>
-    <col min="3" max="3" width="4.625" customWidth="1"/>
-    <col min="4" max="4" width="7.25" customWidth="1"/>
-    <col min="5" max="5" width="6.75" customWidth="1"/>
-    <col min="6" max="6" width="6.25" customWidth="1"/>
-    <col min="7" max="7" width="5.625" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="50" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="48" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="51" t="s">
-        <v>241</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>239</v>
-      </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="48" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="51" t="s">
-        <v>237</v>
-      </c>
-      <c r="F1" s="51" t="s">
+      <c r="G1" s="49" t="s">
         <v>245</v>
       </c>
-      <c r="G1" s="52" t="s">
-        <v>246</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
-        <v>236</v>
+      <c r="A2" s="51" t="s">
+        <v>235</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>234</v>
-      </c>
-      <c r="C2" s="47">
+        <v>233</v>
+      </c>
+      <c r="C2" s="44">
         <v>3</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="44">
+        <v>225</v>
+      </c>
+      <c r="E2" s="41">
         <v>0</v>
       </c>
       <c r="F2" s="18"/>
       <c r="G2" s="23"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="55"/>
+      <c r="A3" s="52"/>
       <c r="B3" s="20"/>
-      <c r="C3" s="48"/>
+      <c r="C3" s="45"/>
       <c r="D3" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="E3" s="45">
+        <v>226</v>
+      </c>
+      <c r="E3" s="42">
         <v>1</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="52"/>
       <c r="B4" s="20"/>
-      <c r="C4" s="48"/>
+      <c r="C4" s="45"/>
       <c r="D4" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="E4" s="45">
+        <v>227</v>
+      </c>
+      <c r="E4" s="42">
         <v>2</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="29"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="52"/>
       <c r="B5" s="20"/>
-      <c r="C5" s="48"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="E5" s="45">
+        <v>228</v>
+      </c>
+      <c r="E5" s="42">
         <v>3</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="29"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="52"/>
       <c r="B6" s="20"/>
-      <c r="C6" s="48"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="E6" s="45">
+        <v>229</v>
+      </c>
+      <c r="E6" s="42">
         <v>4</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
+      <c r="A7" s="52"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="48"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="E7" s="45">
+        <v>230</v>
+      </c>
+      <c r="E7" s="42">
         <v>5</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="29"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
+      <c r="A8" s="52"/>
       <c r="B8" s="20"/>
-      <c r="C8" s="48"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="E8" s="45">
+        <v>231</v>
+      </c>
+      <c r="E8" s="42">
         <v>6</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="29"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="56"/>
+      <c r="A9" s="53"/>
       <c r="B9" s="25"/>
-      <c r="C9" s="49"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="E9" s="46">
+        <v>232</v>
+      </c>
+      <c r="E9" s="43">
         <v>7</v>
       </c>
       <c r="F9" s="25"/>
       <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="s">
-        <v>240</v>
+      <c r="A10" s="51" t="s">
+        <v>239</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="C10" s="47">
+        <v>234</v>
+      </c>
+      <c r="C10" s="44">
         <v>3</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="E10" s="44">
+        <v>225</v>
+      </c>
+      <c r="E10" s="41">
         <v>0</v>
       </c>
       <c r="F10" s="18"/>
       <c r="G10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
+      <c r="A11" s="52"/>
       <c r="B11" s="20"/>
-      <c r="C11" s="48"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="28" t="s">
-        <v>227</v>
-      </c>
-      <c r="E11" s="45">
+        <v>226</v>
+      </c>
+      <c r="E11" s="42">
         <v>1</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="29"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
+      <c r="A12" s="52"/>
       <c r="B12" s="20"/>
-      <c r="C12" s="48"/>
+      <c r="C12" s="45"/>
       <c r="D12" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="E12" s="45">
+        <v>227</v>
+      </c>
+      <c r="E12" s="42">
         <v>2</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="29"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
+      <c r="A13" s="52"/>
       <c r="B13" s="20"/>
-      <c r="C13" s="48"/>
+      <c r="C13" s="45"/>
       <c r="D13" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13" s="45">
+        <v>228</v>
+      </c>
+      <c r="E13" s="42">
         <v>3</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="29"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
+      <c r="A14" s="52"/>
       <c r="B14" s="20"/>
-      <c r="C14" s="48"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="E14" s="45">
+        <v>229</v>
+      </c>
+      <c r="E14" s="42">
         <v>4</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="29"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="20"/>
-      <c r="C15" s="48"/>
+      <c r="C15" s="45"/>
       <c r="D15" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="E15" s="45">
+        <v>230</v>
+      </c>
+      <c r="E15" s="42">
         <v>5</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="29"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="20"/>
-      <c r="C16" s="48"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="E16" s="45">
+        <v>231</v>
+      </c>
+      <c r="E16" s="42">
         <v>6</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="29"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="56"/>
+      <c r="A17" s="53"/>
       <c r="B17" s="25"/>
-      <c r="C17" s="49"/>
+      <c r="C17" s="46"/>
       <c r="D17" s="24" t="s">
-        <v>233</v>
-      </c>
-      <c r="E17" s="46">
+        <v>232</v>
+      </c>
+      <c r="E17" s="43">
         <v>7</v>
       </c>
       <c r="F17" s="25"/>
       <c r="G17" s="27"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="51" t="s">
+        <v>246</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18" s="44">
+        <v>6</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="44">
+        <v>0</v>
+      </c>
+      <c r="G18" s="41">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="52" t="s">
         <v>247</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="C18" s="47">
+      <c r="B19" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C19" s="45">
         <v>6</v>
       </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="47">
-        <v>0</v>
-      </c>
-      <c r="G18" s="44">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="D19" s="28"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="45">
+        <v>-31</v>
+      </c>
+      <c r="G19" s="42">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="52" t="s">
+        <v>241</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="45">
+        <v>8</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="45">
+        <v>0</v>
+      </c>
+      <c r="G20" s="42">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="52" t="s">
         <v>248</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="C19" s="48">
-        <v>6</v>
-      </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="48">
-        <v>-31</v>
-      </c>
-      <c r="G19" s="45">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+      <c r="B21" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="B20" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="C20" s="48">
+      <c r="C21" s="45">
         <v>8</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="48">
-        <v>0</v>
-      </c>
-      <c r="G20" s="45">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="55" t="s">
+      <c r="D21" s="28"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="45">
+        <v>-127</v>
+      </c>
+      <c r="G21" s="42">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="52" t="s">
         <v>249</v>
       </c>
-      <c r="B21" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="C21" s="48">
-        <v>8</v>
-      </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="48">
-        <v>-127</v>
-      </c>
-      <c r="G21" s="45">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="55" t="s">
+      <c r="B22" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="45">
+        <v>12</v>
+      </c>
+      <c r="D22" s="28"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="45">
+        <v>0</v>
+      </c>
+      <c r="G22" s="42">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="53" t="s">
         <v>250</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="C22" s="48">
+      <c r="B23" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="C23" s="46">
         <v>12</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="48">
-        <v>0</v>
-      </c>
-      <c r="G22" s="45">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="D23" s="24"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="46">
+        <v>-2047</v>
+      </c>
+      <c r="G23" s="43">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="51" t="s">
         <v>251</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>243</v>
-      </c>
-      <c r="C23" s="49">
-        <v>12</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="49">
-        <v>-2047</v>
-      </c>
-      <c r="G23" s="46">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="54" t="s">
+      <c r="B24" s="18" t="s">
         <v>252</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="C24" s="44">
+        <v>1</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="C24" s="47">
-        <v>1</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="E24" s="44">
+      <c r="E24" s="41">
         <v>0</v>
       </c>
       <c r="F24" s="18"/>
       <c r="G24" s="23"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
+      <c r="A25" s="53"/>
       <c r="B25" s="25"/>
-      <c r="C25" s="49"/>
+      <c r="C25" s="46"/>
       <c r="D25" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="E25" s="46">
+        <v>254</v>
+      </c>
+      <c r="E25" s="43">
         <v>1</v>
       </c>
       <c r="F25" s="25"/>
       <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="51" t="s">
+        <v>257</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="B26" s="18" t="s">
-        <v>259</v>
-      </c>
-      <c r="C26" s="47">
+      <c r="C26" s="44">
         <v>3</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="E26" s="44">
+        <v>260</v>
+      </c>
+      <c r="E26" s="41">
         <v>0</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
+      <c r="A27" s="52"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="48"/>
+      <c r="C27" s="45"/>
       <c r="D27" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="E27" s="45">
+        <v>261</v>
+      </c>
+      <c r="E27" s="42">
         <v>1</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="29"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
+      <c r="A28" s="52"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="48"/>
+      <c r="C28" s="45"/>
       <c r="D28" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="E28" s="45">
+        <v>259</v>
+      </c>
+      <c r="E28" s="42">
         <v>2</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="29"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
+      <c r="A29" s="52"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="48"/>
+      <c r="C29" s="45"/>
       <c r="D29" s="28" t="s">
-        <v>263</v>
-      </c>
-      <c r="E29" s="45">
+        <v>262</v>
+      </c>
+      <c r="E29" s="42">
         <v>3</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="29"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
+      <c r="A30" s="52"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="48"/>
+      <c r="C30" s="45"/>
       <c r="D30" s="28" t="s">
-        <v>254</v>
-      </c>
-      <c r="E30" s="45">
+        <v>253</v>
+      </c>
+      <c r="E30" s="42">
         <v>4</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="29"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
+      <c r="A31" s="52"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="48"/>
+      <c r="C31" s="45"/>
       <c r="D31" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="E31" s="45">
+        <v>254</v>
+      </c>
+      <c r="E31" s="42">
         <v>5</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="29"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="56"/>
+      <c r="A32" s="53"/>
       <c r="B32" s="25"/>
-      <c r="C32" s="49"/>
+      <c r="C32" s="46"/>
       <c r="D32" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="E32" s="46">
+        <v>263</v>
+      </c>
+      <c r="E32" s="43">
         <v>6</v>
       </c>
       <c r="F32" s="25"/>
       <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="54" t="s">
+      <c r="A33" s="51" t="s">
+        <v>264</v>
+      </c>
+      <c r="B33" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="C33" s="47">
+      <c r="C33" s="44">
         <v>3</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="E33" s="44">
+        <v>260</v>
+      </c>
+      <c r="E33" s="41">
         <v>0</v>
       </c>
       <c r="F33" s="18"/>
       <c r="G33" s="23"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
+      <c r="A34" s="52"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="48"/>
+      <c r="C34" s="45"/>
       <c r="D34" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="E34" s="45">
+        <v>261</v>
+      </c>
+      <c r="E34" s="42">
         <v>1</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="29"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
+      <c r="A35" s="52"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="48"/>
+      <c r="C35" s="45"/>
       <c r="D35" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="E35" s="45">
+        <v>259</v>
+      </c>
+      <c r="E35" s="42">
         <v>2</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="29"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="55"/>
+      <c r="A36" s="52"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="48"/>
+      <c r="C36" s="45"/>
       <c r="D36" s="28" t="s">
-        <v>263</v>
-      </c>
-      <c r="E36" s="45">
+        <v>262</v>
+      </c>
+      <c r="E36" s="42">
         <v>3</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="29"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
+      <c r="A37" s="52"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="48"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="28" t="s">
-        <v>254</v>
-      </c>
-      <c r="E37" s="45">
+        <v>253</v>
+      </c>
+      <c r="E37" s="42">
         <v>4</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="29"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="55"/>
+      <c r="A38" s="52"/>
       <c r="B38" s="20"/>
-      <c r="C38" s="48"/>
+      <c r="C38" s="45"/>
       <c r="D38" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="E38" s="45">
+        <v>254</v>
+      </c>
+      <c r="E38" s="42">
         <v>5</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="29"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
+      <c r="A39" s="53"/>
       <c r="B39" s="25"/>
-      <c r="C39" s="49"/>
+      <c r="C39" s="46"/>
       <c r="D39" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="E39" s="46">
+        <v>263</v>
+      </c>
+      <c r="E39" s="43">
         <v>6</v>
       </c>
       <c r="F39" s="25"/>
       <c r="G39" s="27"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
-        <v>256</v>
+      <c r="A40" s="54" t="s">
+        <v>255</v>
       </c>
       <c r="B40" s="31"/>
-      <c r="C40" s="50"/>
+      <c r="C40" s="47"/>
       <c r="D40" s="30"/>
       <c r="E40" s="33"/>
       <c r="F40" s="31"/>
@@ -5067,15 +5067,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5149,7 +5149,7 @@
         <v>107</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
@@ -5193,7 +5193,7 @@
         <v>116</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>22</v>
@@ -5303,7 +5303,7 @@
         <v>155</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>98</v>
@@ -5410,13 +5410,13 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5432,13 +5432,13 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5461,15 +5461,15 @@
       </c>
       <c r="C35" s="9"/>
     </row>
-    <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5485,24 +5485,24 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>89</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5518,13 +5518,13 @@
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5535,18 +5535,18 @@
         <v>51</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>138</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5560,158 +5560,158 @@
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C45" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="11" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>274</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>141</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>112</v>
       </c>
       <c r="C48" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="11" t="s">
         <v>279</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
-        <v>280</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>146</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>145</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>144</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>113</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>147</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>149</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C56" s="9" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="11" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="11" t="s">
-        <v>294</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>151</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>152</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5736,7 +5736,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
         <v>172</v>
       </c>

</xml_diff>

<commit_message>
generate all permutations of microinstructions
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="318">
   <si>
     <t>Instruction</t>
   </si>
@@ -287,15 +287,9 @@
     <t>Load Displacement from Program</t>
   </si>
   <si>
-    <t>PUSHS SPEC</t>
-  </si>
-  <si>
     <t>Push Special Register</t>
   </si>
   <si>
-    <t>POPS  SPEC</t>
-  </si>
-  <si>
     <t>Pop Special Register</t>
   </si>
   <si>
@@ -671,12 +665,6 @@
     <t>MDR = PC</t>
   </si>
   <si>
-    <t>MDR = SPEC</t>
-  </si>
-  <si>
-    <t>SPEC = MDR</t>
-  </si>
-  <si>
     <t>PC = MDR</t>
   </si>
   <si>
@@ -987,6 +975,12 @@
   </si>
   <si>
     <t xml:space="preserve">0xFF - DST </t>
+  </si>
+  <si>
+    <t>MDR = SPC</t>
+  </si>
+  <si>
+    <t>SPC = MDR</t>
   </si>
 </sst>
 </file>
@@ -1313,7 +1307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1404,6 +1398,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1810,8 +1805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,16 +1826,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D1" s="35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1848,11 +1843,11 @@
         <v>55</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E2" s="23">
         <v>1</v>
@@ -1860,14 +1855,14 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E3" s="23">
         <v>1</v>
@@ -1878,11 +1873,11 @@
         <v>3</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E4" s="33">
         <v>1</v>
@@ -1893,11 +1888,11 @@
         <v>6</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E5" s="33">
         <v>1</v>
@@ -1908,11 +1903,11 @@
         <v>9</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E6" s="33">
         <v>1</v>
@@ -1920,14 +1915,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E7" s="33">
         <v>1</v>
@@ -1938,11 +1933,11 @@
         <v>13</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E8" s="33">
         <v>1</v>
@@ -1953,11 +1948,11 @@
         <v>16</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E9" s="33">
         <v>1</v>
@@ -1968,11 +1963,11 @@
         <v>19</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E10" s="33">
         <v>1</v>
@@ -1980,14 +1975,14 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E11" s="33">
         <v>1</v>
@@ -1998,11 +1993,11 @@
         <v>23</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E12" s="33">
         <v>1</v>
@@ -2013,11 +2008,11 @@
         <v>9</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E13" s="33">
         <v>1</v>
@@ -2028,11 +2023,11 @@
         <v>28</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E14" s="33">
         <v>1</v>
@@ -2043,11 +2038,11 @@
         <v>31</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E15" s="33">
         <v>1</v>
@@ -2058,11 +2053,11 @@
         <v>34</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E16" s="33">
         <v>1</v>
@@ -2073,11 +2068,11 @@
         <v>37</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E17" s="33">
         <v>1</v>
@@ -2085,14 +2080,14 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E18" s="33">
         <v>1</v>
@@ -2100,14 +2095,14 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E19" s="33">
         <v>1</v>
@@ -2115,14 +2110,14 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E20" s="33">
         <v>1</v>
@@ -2130,14 +2125,14 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E21" s="33">
         <v>1</v>
@@ -2148,11 +2143,11 @@
         <v>40</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E22" s="33">
         <v>1</v>
@@ -2163,11 +2158,11 @@
         <v>43</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E23" s="23">
         <v>1</v>
@@ -2178,7 +2173,7 @@
         <v>68</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -2189,13 +2184,13 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
       <c r="B25" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>200</v>
-      </c>
       <c r="D25" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E25" s="27">
         <v>0</v>
@@ -2206,10 +2201,10 @@
         <v>71</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="23">
@@ -2219,11 +2214,11 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
       <c r="B27" s="26" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E27" s="27">
         <v>0</v>
@@ -2234,11 +2229,11 @@
         <v>74</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E28" s="33">
         <v>1</v>
@@ -2249,11 +2244,11 @@
         <v>77</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E29" s="33">
         <v>1</v>
@@ -2261,14 +2256,14 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="38" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E30" s="33">
         <v>1</v>
@@ -2276,14 +2271,14 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E31" s="33">
         <v>1</v>
@@ -2291,14 +2286,14 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E32" s="33">
         <v>1</v>
@@ -2306,13 +2301,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="23">
@@ -2322,11 +2317,11 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="39"/>
       <c r="B34" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E34" s="27">
         <v>0</v>
@@ -2337,10 +2332,10 @@
         <v>60</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="23">
@@ -2350,11 +2345,11 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="39"/>
       <c r="B36" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E36" s="27">
         <v>0</v>
@@ -2362,10 +2357,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -2376,13 +2371,13 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="39"/>
       <c r="B38" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E38" s="27">
         <v>0</v>
@@ -2393,7 +2388,7 @@
         <v>64</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>305</v>
+        <v>207</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -2404,13 +2399,13 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="39"/>
       <c r="B40" s="26" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E40" s="27">
         <v>0</v>
@@ -2427,13 +2422,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>209</v>
+        <v>301</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="23">
@@ -2443,11 +2438,11 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="39"/>
       <c r="B43" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E43" s="27">
         <v>0</v>
@@ -2458,10 +2453,10 @@
         <v>82</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="23">
@@ -2471,11 +2466,11 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="39"/>
       <c r="B45" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E45" s="27">
         <v>0</v>
@@ -2483,10 +2478,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="37" t="s">
-        <v>86</v>
+        <v>218</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -2497,13 +2492,13 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="39"/>
       <c r="B47" s="26" t="s">
-        <v>214</v>
+        <v>316</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E47" s="27">
         <v>0</v>
@@ -2511,13 +2506,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
-        <v>88</v>
+        <v>217</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D48" s="18"/>
       <c r="E48" s="23">
@@ -2527,11 +2522,11 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="39"/>
       <c r="B49" s="26" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C49" s="25"/>
       <c r="D49" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E49" s="27">
         <v>0</v>
@@ -2541,12 +2536,12 @@
       <c r="A50" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="B50" s="32" t="s">
-        <v>212</v>
+      <c r="B50" s="58" t="s">
+        <v>210</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E50" s="33">
         <v>0</v>
@@ -2554,14 +2549,14 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="38" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E51" s="33">
         <v>0</v>
@@ -2572,7 +2567,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -2583,7 +2578,7 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="21" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C53" s="20"/>
       <c r="D53" s="20"/>
@@ -2594,11 +2589,11 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="39"/>
       <c r="B54" s="26" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E54" s="27">
         <v>0</v>
@@ -2606,10 +2601,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="37" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2620,9 +2615,11 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="C56" s="20"/>
+        <v>211</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>198</v>
+      </c>
       <c r="D56" s="20"/>
       <c r="E56" s="29">
         <v>0</v>
@@ -2631,11 +2628,11 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="39"/>
       <c r="B57" s="26" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E57" s="27">
         <v>0</v>
@@ -2646,10 +2643,10 @@
         <v>52</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="23">
@@ -2659,11 +2656,11 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="39"/>
       <c r="B59" s="26" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E59" s="27">
         <v>0</v>
@@ -2671,14 +2668,14 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="38" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E60" s="33">
         <v>0</v>
@@ -2686,14 +2683,14 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="38" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E61" s="33">
         <v>0</v>
@@ -2701,14 +2698,14 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="38" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E62" s="33">
         <v>0</v>
@@ -2716,14 +2713,14 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="38" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E63" s="33">
         <v>0</v>
@@ -2731,14 +2728,14 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="38" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E64" s="33">
         <v>0</v>
@@ -2746,14 +2743,14 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="38" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E65" s="33">
         <v>0</v>
@@ -2761,14 +2758,14 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="38" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E66" s="33">
         <v>0</v>
@@ -2776,14 +2773,14 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="38" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E67" s="33">
         <v>0</v>
@@ -2791,14 +2788,14 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="38" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E68" s="33">
         <v>0</v>
@@ -2806,14 +2803,14 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="38" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C69" s="31"/>
       <c r="D69" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E69" s="33">
         <v>0</v>
@@ -2821,14 +2818,14 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="38" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E70" s="33">
         <v>0</v>
@@ -2836,14 +2833,14 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="38" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E71" s="33">
         <v>0</v>
@@ -2851,14 +2848,14 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="38" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E72" s="33">
         <v>0</v>
@@ -2866,14 +2863,14 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="38" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E73" s="33">
         <v>0</v>
@@ -2881,14 +2878,14 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C74" s="31"/>
       <c r="D74" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E74" s="33">
         <v>0</v>
@@ -2896,14 +2893,14 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E75" s="33">
         <v>0</v>
@@ -2911,14 +2908,14 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E76" s="33">
         <v>0</v>
@@ -2926,14 +2923,14 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="38" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C77" s="31"/>
       <c r="D77" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E77" s="33">
         <v>0</v>
@@ -2941,14 +2938,14 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B78" s="32" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="31" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E78" s="33">
         <v>0</v>
@@ -2964,18 +2961,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:C63"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="7" width="4.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="7" width="5.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2989,13 +2986,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E1" s="55"/>
       <c r="F1" s="55"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I1" s="55"/>
     </row>
@@ -3010,21 +3007,21 @@
         <v>57</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>58</v>
@@ -3033,22 +3030,22 @@
         <v>59</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H3" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3062,16 +3059,16 @@
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3085,16 +3082,16 @@
         <v>8</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3108,51 +3105,51 @@
         <v>11</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F6" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H6" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H7" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3166,16 +3163,16 @@
         <v>15</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3189,16 +3186,16 @@
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3212,51 +3209,51 @@
         <v>21</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H10" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H11" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3270,16 +3267,16 @@
         <v>25</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3293,22 +3290,22 @@
         <v>27</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3322,16 +3319,16 @@
         <v>30</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3345,22 +3342,22 @@
         <v>33</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F15" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H15" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3374,16 +3371,16 @@
         <v>36</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3397,126 +3394,126 @@
         <v>39</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F17" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H17" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>92</v>
-      </c>
       <c r="D18" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="D19" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F20" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G20" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H20" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="H21" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3530,10 +3527,10 @@
         <v>42</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3547,10 +3544,10 @@
         <v>45</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3564,10 +3561,10 @@
         <v>70</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3581,10 +3578,10 @@
         <v>73</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3598,10 +3595,10 @@
         <v>76</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3615,84 +3612,84 @@
         <v>79</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="C28" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="C29" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="H30" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" s="5" t="s">
         <v>100</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3706,45 +3703,45 @@
         <v>62</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3758,22 +3755,22 @@
         <v>66</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3785,33 +3782,33 @@
       </c>
       <c r="C35" s="9"/>
       <c r="H35" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3825,56 +3822,56 @@
         <v>84</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3888,39 +3885,39 @@
         <v>49</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3931,42 +3928,42 @@
         <v>51</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3980,459 +3977,459 @@
         <v>54</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="E46" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>274</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>143</v>
-      </c>
       <c r="F46" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G46" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G47" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D49" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G49" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G50" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G51" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F52" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F53" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G54" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G55" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G56" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="D59" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F59" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="G59" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="G59" s="10" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="D60" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C61" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G60" s="8" t="s">
+      <c r="D61" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H60" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="E61" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="F61" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B62" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>171</v>
-      </c>
       <c r="D62" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E62" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G62" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4449,8 +4446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4466,39 +4463,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B1" s="48" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>232</v>
+      </c>
+      <c r="F1" s="48" t="s">
         <v>240</v>
       </c>
-      <c r="C1" s="48" t="s">
-        <v>238</v>
-      </c>
-      <c r="D1" s="48" t="s">
-        <v>243</v>
-      </c>
-      <c r="E1" s="48" t="s">
-        <v>236</v>
-      </c>
-      <c r="F1" s="48" t="s">
-        <v>244</v>
-      </c>
       <c r="G1" s="49" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C2" s="44">
         <v>3</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E2" s="41">
         <v>0</v>
@@ -4511,7 +4508,7 @@
       <c r="B3" s="20"/>
       <c r="C3" s="45"/>
       <c r="D3" s="28" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E3" s="42">
         <v>1</v>
@@ -4524,7 +4521,7 @@
       <c r="B4" s="20"/>
       <c r="C4" s="45"/>
       <c r="D4" s="28" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E4" s="42">
         <v>2</v>
@@ -4537,7 +4534,7 @@
       <c r="B5" s="20"/>
       <c r="C5" s="45"/>
       <c r="D5" s="28" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E5" s="42">
         <v>3</v>
@@ -4550,7 +4547,7 @@
       <c r="B6" s="20"/>
       <c r="C6" s="45"/>
       <c r="D6" s="28" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E6" s="42">
         <v>4</v>
@@ -4563,7 +4560,7 @@
       <c r="B7" s="20"/>
       <c r="C7" s="45"/>
       <c r="D7" s="28" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E7" s="42">
         <v>5</v>
@@ -4576,7 +4573,7 @@
       <c r="B8" s="20"/>
       <c r="C8" s="45"/>
       <c r="D8" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E8" s="42">
         <v>6</v>
@@ -4589,7 +4586,7 @@
       <c r="B9" s="25"/>
       <c r="C9" s="46"/>
       <c r="D9" s="24" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E9" s="43">
         <v>7</v>
@@ -4599,16 +4596,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C10" s="44">
         <v>3</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E10" s="41">
         <v>0</v>
@@ -4621,7 +4618,7 @@
       <c r="B11" s="20"/>
       <c r="C11" s="45"/>
       <c r="D11" s="28" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E11" s="42">
         <v>1</v>
@@ -4634,7 +4631,7 @@
       <c r="B12" s="20"/>
       <c r="C12" s="45"/>
       <c r="D12" s="28" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E12" s="42">
         <v>2</v>
@@ -4647,7 +4644,7 @@
       <c r="B13" s="20"/>
       <c r="C13" s="45"/>
       <c r="D13" s="28" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E13" s="42">
         <v>3</v>
@@ -4660,7 +4657,7 @@
       <c r="B14" s="20"/>
       <c r="C14" s="45"/>
       <c r="D14" s="28" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E14" s="42">
         <v>4</v>
@@ -4673,7 +4670,7 @@
       <c r="B15" s="20"/>
       <c r="C15" s="45"/>
       <c r="D15" s="28" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E15" s="42">
         <v>5</v>
@@ -4686,7 +4683,7 @@
       <c r="B16" s="20"/>
       <c r="C16" s="45"/>
       <c r="D16" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E16" s="42">
         <v>6</v>
@@ -4699,7 +4696,7 @@
       <c r="B17" s="25"/>
       <c r="C17" s="46"/>
       <c r="D17" s="24" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E17" s="43">
         <v>7</v>
@@ -4709,10 +4706,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="51" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C18" s="44">
         <v>6</v>
@@ -4728,10 +4725,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C19" s="45">
         <v>6</v>
@@ -4747,10 +4744,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C20" s="45">
         <v>8</v>
@@ -4766,10 +4763,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C21" s="45">
         <v>8</v>
@@ -4785,10 +4782,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C22" s="45">
         <v>12</v>
@@ -4804,10 +4801,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C23" s="46">
         <v>12</v>
@@ -4823,16 +4820,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C24" s="44">
         <v>1</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E24" s="41">
         <v>0</v>
@@ -4845,7 +4842,7 @@
       <c r="B25" s="25"/>
       <c r="C25" s="46"/>
       <c r="D25" s="24" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E25" s="43">
         <v>1</v>
@@ -4855,16 +4852,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C26" s="44">
         <v>3</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E26" s="41">
         <v>0</v>
@@ -4877,7 +4874,7 @@
       <c r="B27" s="20"/>
       <c r="C27" s="45"/>
       <c r="D27" s="28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E27" s="42">
         <v>1</v>
@@ -4890,7 +4887,7 @@
       <c r="B28" s="20"/>
       <c r="C28" s="45"/>
       <c r="D28" s="28" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E28" s="42">
         <v>2</v>
@@ -4903,7 +4900,7 @@
       <c r="B29" s="20"/>
       <c r="C29" s="45"/>
       <c r="D29" s="28" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E29" s="42">
         <v>3</v>
@@ -4916,7 +4913,7 @@
       <c r="B30" s="20"/>
       <c r="C30" s="45"/>
       <c r="D30" s="28" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E30" s="42">
         <v>4</v>
@@ -4929,7 +4926,7 @@
       <c r="B31" s="20"/>
       <c r="C31" s="45"/>
       <c r="D31" s="28" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E31" s="42">
         <v>5</v>
@@ -4942,7 +4939,7 @@
       <c r="B32" s="25"/>
       <c r="C32" s="46"/>
       <c r="D32" s="24" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E32" s="43">
         <v>6</v>
@@ -4952,16 +4949,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="51" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C33" s="44">
         <v>3</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E33" s="41">
         <v>0</v>
@@ -4974,7 +4971,7 @@
       <c r="B34" s="20"/>
       <c r="C34" s="45"/>
       <c r="D34" s="28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="E34" s="42">
         <v>1</v>
@@ -4987,7 +4984,7 @@
       <c r="B35" s="20"/>
       <c r="C35" s="45"/>
       <c r="D35" s="28" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E35" s="42">
         <v>2</v>
@@ -5000,7 +4997,7 @@
       <c r="B36" s="20"/>
       <c r="C36" s="45"/>
       <c r="D36" s="28" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E36" s="42">
         <v>3</v>
@@ -5013,7 +5010,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="45"/>
       <c r="D37" s="28" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E37" s="42">
         <v>4</v>
@@ -5026,7 +5023,7 @@
       <c r="B38" s="20"/>
       <c r="C38" s="45"/>
       <c r="D38" s="28" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E38" s="42">
         <v>5</v>
@@ -5039,7 +5036,7 @@
       <c r="B39" s="25"/>
       <c r="C39" s="46"/>
       <c r="D39" s="24" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E39" s="43">
         <v>6</v>
@@ -5049,7 +5046,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="54" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="47"/>
@@ -5102,7 +5099,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>58</v>
@@ -5146,10 +5143,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
@@ -5190,10 +5187,10 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>22</v>
@@ -5267,46 +5264,46 @@
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>90</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>93</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5377,46 +5374,46 @@
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>125</v>
-      </c>
       <c r="C28" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>126</v>
-      </c>
       <c r="C29" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5432,13 +5429,13 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5463,13 +5460,13 @@
     </row>
     <row r="36" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5485,24 +5482,24 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5518,13 +5515,13 @@
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5535,18 +5532,18 @@
         <v>51</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5562,211 +5559,211 @@
     </row>
     <row r="45" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C59" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C60" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
encodes all possible alu operations
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="316">
   <si>
     <t>Instruction</t>
   </si>
@@ -587,18 +587,6 @@
     <t>DST = DST ^ IMM8</t>
   </si>
   <si>
-    <t>DST - SRC</t>
-  </si>
-  <si>
-    <t>DST - SRC - C</t>
-  </si>
-  <si>
-    <t>DST - IMM8</t>
-  </si>
-  <si>
-    <t>DST - IMM8 - C</t>
-  </si>
-  <si>
     <t>0x00 - DST</t>
   </si>
   <si>
@@ -617,9 +605,6 @@
     <t>MAR = SP = SP - 1</t>
   </si>
   <si>
-    <t>MDR = DST</t>
-  </si>
-  <si>
     <t>Memory</t>
   </si>
   <si>
@@ -635,9 +620,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>DST = DST &lt;&lt; 1</t>
-  </si>
-  <si>
     <t>DST = DST &gt;&gt; 1</t>
   </si>
   <si>
@@ -647,24 +629,15 @@
     <t>DST = DST - 1</t>
   </si>
   <si>
-    <t>DST &amp; DST</t>
-  </si>
-  <si>
     <t>MAR = IMM12</t>
   </si>
   <si>
     <t>MDR = SRC</t>
   </si>
   <si>
-    <t>SRC = MDR</t>
-  </si>
-  <si>
     <t>PC = IMM12</t>
   </si>
   <si>
-    <t>MDR = PC</t>
-  </si>
-  <si>
     <t>PC = MDR</t>
   </si>
   <si>
@@ -981,6 +954,27 @@
   </si>
   <si>
     <t>SPC = MDR</t>
+  </si>
+  <si>
+    <t>MDR = PC + 2</t>
+  </si>
+  <si>
+    <t>-31</t>
+  </si>
+  <si>
+    <t>REG - IMM8</t>
+  </si>
+  <si>
+    <t>REG - IMM8 - C</t>
+  </si>
+  <si>
+    <t>REG1 - REG2 - C</t>
+  </si>
+  <si>
+    <t>REG1 - REG2</t>
+  </si>
+  <si>
+    <t>DST = DST + DST</t>
   </si>
 </sst>
 </file>
@@ -1805,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,16 +1820,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="C1" s="35" t="s">
-        <v>197</v>
-      </c>
       <c r="D1" s="35" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1847,7 +1841,7 @@
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E2" s="23">
         <v>1</v>
@@ -1862,7 +1856,7 @@
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E3" s="23">
         <v>1</v>
@@ -1877,7 +1871,7 @@
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E4" s="33">
         <v>1</v>
@@ -1892,7 +1886,7 @@
       </c>
       <c r="C5" s="31"/>
       <c r="D5" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E5" s="33">
         <v>1</v>
@@ -1907,7 +1901,7 @@
       </c>
       <c r="C6" s="31"/>
       <c r="D6" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E6" s="33">
         <v>1</v>
@@ -1922,7 +1916,7 @@
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E7" s="33">
         <v>1</v>
@@ -1937,7 +1931,7 @@
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E8" s="33">
         <v>1</v>
@@ -1952,7 +1946,7 @@
       </c>
       <c r="C9" s="31"/>
       <c r="D9" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E9" s="33">
         <v>1</v>
@@ -1967,7 +1961,7 @@
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E10" s="33">
         <v>1</v>
@@ -1982,7 +1976,7 @@
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E11" s="33">
         <v>1</v>
@@ -1997,7 +1991,7 @@
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E12" s="33">
         <v>1</v>
@@ -2012,7 +2006,7 @@
       </c>
       <c r="C13" s="31"/>
       <c r="D13" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E13" s="33">
         <v>1</v>
@@ -2027,7 +2021,7 @@
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E14" s="33">
         <v>1</v>
@@ -2042,7 +2036,7 @@
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E15" s="33">
         <v>1</v>
@@ -2057,7 +2051,7 @@
       </c>
       <c r="C16" s="31"/>
       <c r="D16" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E16" s="33">
         <v>1</v>
@@ -2072,7 +2066,7 @@
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E17" s="33">
         <v>1</v>
@@ -2083,11 +2077,11 @@
         <v>88</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>186</v>
+        <v>314</v>
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E18" s="33">
         <v>1</v>
@@ -2098,11 +2092,11 @@
         <v>91</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>187</v>
+        <v>313</v>
       </c>
       <c r="C19" s="31"/>
       <c r="D19" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E19" s="33">
         <v>1</v>
@@ -2113,11 +2107,11 @@
         <v>120</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>188</v>
+        <v>311</v>
       </c>
       <c r="C20" s="31"/>
       <c r="D20" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E20" s="33">
         <v>1</v>
@@ -2128,11 +2122,11 @@
         <v>153</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>189</v>
+        <v>312</v>
       </c>
       <c r="C21" s="31"/>
       <c r="D21" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E21" s="33">
         <v>1</v>
@@ -2143,11 +2137,11 @@
         <v>40</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C22" s="31"/>
       <c r="D22" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E22" s="33">
         <v>1</v>
@@ -2158,11 +2152,11 @@
         <v>43</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C23" s="18"/>
       <c r="D23" s="18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E23" s="23">
         <v>1</v>
@@ -2173,7 +2167,7 @@
         <v>68</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="18"/>
@@ -2184,13 +2178,13 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="39"/>
       <c r="B25" s="26" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E25" s="27">
         <v>0</v>
@@ -2201,10 +2195,10 @@
         <v>71</v>
       </c>
       <c r="B26" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>194</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>199</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="23">
@@ -2214,11 +2208,11 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="39"/>
       <c r="B27" s="26" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="C27" s="25"/>
       <c r="D27" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E27" s="27">
         <v>0</v>
@@ -2229,11 +2223,11 @@
         <v>74</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>202</v>
+        <v>315</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E28" s="33">
         <v>1</v>
@@ -2244,11 +2238,11 @@
         <v>77</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C29" s="31"/>
       <c r="D29" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E29" s="33">
         <v>1</v>
@@ -2259,11 +2253,11 @@
         <v>121</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C30" s="31"/>
       <c r="D30" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E30" s="33">
         <v>1</v>
@@ -2274,11 +2268,11 @@
         <v>122</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C31" s="31"/>
       <c r="D31" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E31" s="33">
         <v>1</v>
@@ -2289,11 +2283,11 @@
         <v>97</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>206</v>
+        <v>99</v>
       </c>
       <c r="C32" s="31"/>
       <c r="D32" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E32" s="33">
         <v>1</v>
@@ -2301,13 +2295,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="37" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="23">
@@ -2317,11 +2311,11 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="39"/>
       <c r="B34" s="26" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C34" s="25"/>
       <c r="D34" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E34" s="27">
         <v>0</v>
@@ -2332,10 +2326,10 @@
         <v>60</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="23">
@@ -2345,11 +2339,11 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="39"/>
       <c r="B36" s="26" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C36" s="25"/>
       <c r="D36" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E36" s="27">
         <v>0</v>
@@ -2357,10 +2351,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="37" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -2371,13 +2365,13 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="39"/>
       <c r="B38" s="26" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D38" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E38" s="27">
         <v>0</v>
@@ -2388,7 +2382,7 @@
         <v>64</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -2399,13 +2393,13 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="39"/>
       <c r="B40" s="26" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E40" s="27">
         <v>0</v>
@@ -2422,13 +2416,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="37" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="23">
@@ -2438,11 +2432,11 @@
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="39"/>
       <c r="B43" s="26" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E43" s="27">
         <v>0</v>
@@ -2453,10 +2447,10 @@
         <v>82</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="C44" s="18" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="23">
@@ -2466,11 +2460,11 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="39"/>
       <c r="B45" s="26" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C45" s="25"/>
       <c r="D45" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E45" s="27">
         <v>0</v>
@@ -2478,10 +2472,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="37" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -2492,13 +2486,13 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="39"/>
       <c r="B47" s="26" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E47" s="27">
         <v>0</v>
@@ -2506,13 +2500,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B48" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C48" s="18" t="s">
         <v>194</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>199</v>
       </c>
       <c r="D48" s="18"/>
       <c r="E48" s="23">
@@ -2522,11 +2516,11 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="39"/>
       <c r="B49" s="26" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="C49" s="25"/>
       <c r="D49" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E49" s="27">
         <v>0</v>
@@ -2537,11 +2531,11 @@
         <v>47</v>
       </c>
       <c r="B50" s="58" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E50" s="33">
         <v>0</v>
@@ -2549,14 +2543,14 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="38" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C51" s="31"/>
       <c r="D51" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E51" s="33">
         <v>0</v>
@@ -2567,7 +2561,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
@@ -2578,9 +2572,11 @@
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="C53" s="20"/>
+        <v>309</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>193</v>
+      </c>
       <c r="D53" s="20"/>
       <c r="E53" s="29">
         <v>0</v>
@@ -2589,11 +2585,11 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="39"/>
       <c r="B54" s="26" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C54" s="25"/>
       <c r="D54" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E54" s="27">
         <v>0</v>
@@ -2601,10 +2597,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="37" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2615,10 +2611,10 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="21" t="s">
-        <v>211</v>
+        <v>309</v>
       </c>
       <c r="C56" s="20" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D56" s="20"/>
       <c r="E56" s="29">
@@ -2628,11 +2624,11 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="39"/>
       <c r="B57" s="26" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C57" s="25"/>
       <c r="D57" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E57" s="27">
         <v>0</v>
@@ -2643,10 +2639,10 @@
         <v>52</v>
       </c>
       <c r="B58" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C58" s="18" t="s">
         <v>194</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>199</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="23">
@@ -2656,11 +2652,11 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="39"/>
       <c r="B59" s="26" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C59" s="25"/>
       <c r="D59" s="25" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E59" s="27">
         <v>0</v>
@@ -2668,14 +2664,14 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="38" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="C60" s="31"/>
       <c r="D60" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E60" s="33">
         <v>0</v>
@@ -2683,14 +2679,14 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="38" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C61" s="31"/>
       <c r="D61" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E61" s="33">
         <v>0</v>
@@ -2698,14 +2694,14 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="38" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C62" s="31"/>
       <c r="D62" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E62" s="33">
         <v>0</v>
@@ -2713,14 +2709,14 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="38" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C63" s="31"/>
       <c r="D63" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E63" s="33">
         <v>0</v>
@@ -2728,14 +2724,14 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="38" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C64" s="31"/>
       <c r="D64" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E64" s="33">
         <v>0</v>
@@ -2743,14 +2739,14 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="38" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C65" s="31"/>
       <c r="D65" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E65" s="33">
         <v>0</v>
@@ -2758,14 +2754,14 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="38" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C66" s="31"/>
       <c r="D66" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E66" s="33">
         <v>0</v>
@@ -2773,14 +2769,14 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="38" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B67" s="32" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C67" s="31"/>
       <c r="D67" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E67" s="33">
         <v>0</v>
@@ -2788,14 +2784,14 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="38" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C68" s="31"/>
       <c r="D68" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E68" s="33">
         <v>0</v>
@@ -2803,14 +2799,14 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="38" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B69" s="32" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="C69" s="31"/>
       <c r="D69" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E69" s="33">
         <v>0</v>
@@ -2818,14 +2814,14 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="38" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C70" s="31"/>
       <c r="D70" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E70" s="33">
         <v>0</v>
@@ -2833,14 +2829,14 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="38" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B71" s="32" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="C71" s="31"/>
       <c r="D71" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E71" s="33">
         <v>0</v>
@@ -2848,14 +2844,14 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="38" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C72" s="31"/>
       <c r="D72" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E72" s="33">
         <v>0</v>
@@ -2863,14 +2859,14 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="38" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B73" s="32" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="C73" s="31"/>
       <c r="D73" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E73" s="33">
         <v>0</v>
@@ -2881,11 +2877,11 @@
         <v>157</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C74" s="31"/>
       <c r="D74" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E74" s="33">
         <v>0</v>
@@ -2896,11 +2892,11 @@
         <v>162</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C75" s="31"/>
       <c r="D75" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E75" s="33">
         <v>0</v>
@@ -2911,11 +2907,11 @@
         <v>170</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C76" s="31"/>
       <c r="D76" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E76" s="33">
         <v>0</v>
@@ -2926,11 +2922,11 @@
         <v>167</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C77" s="31"/>
       <c r="D77" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E77" s="33">
         <v>0</v>
@@ -2945,7 +2941,7 @@
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E78" s="33">
         <v>0</v>
@@ -2961,8 +2957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E48" sqref="E47:E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3128,7 +3124,7 @@
         <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
@@ -3232,7 +3228,7 @@
         <v>114</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>22</v>
@@ -3492,7 +3488,7 @@
         <v>153</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>96</v>
@@ -3671,13 +3667,13 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>106</v>
@@ -3723,13 +3719,13 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>106</v>
@@ -3790,13 +3786,13 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>106</v>
@@ -3842,30 +3838,30 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>134</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>134</v>
@@ -3899,13 +3895,13 @@
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>103</v>
@@ -3928,7 +3924,7 @@
         <v>51</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>116</v>
@@ -3945,13 +3941,13 @@
     </row>
     <row r="43" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="D43" s="8" t="s">
         <v>103</v>
@@ -3985,13 +3981,13 @@
     </row>
     <row r="45" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>137</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="D45" s="8" t="s">
         <v>109</v>
@@ -4008,13 +4004,13 @@
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>109</v>
@@ -4031,13 +4027,13 @@
     </row>
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>140</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D47" s="8" t="s">
         <v>109</v>
@@ -4054,13 +4050,13 @@
     </row>
     <row r="48" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D48" s="8" t="s">
         <v>109</v>
@@ -4077,13 +4073,13 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>144</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>109</v>
@@ -4100,13 +4096,13 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>143</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>109</v>
@@ -4123,13 +4119,13 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>109</v>
@@ -4146,13 +4142,13 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>109</v>
@@ -4169,13 +4165,13 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>145</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>109</v>
@@ -4192,13 +4188,13 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>146</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>109</v>
@@ -4215,13 +4211,13 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>147</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="D55" s="8" t="s">
         <v>109</v>
@@ -4238,13 +4234,13 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>109</v>
@@ -4261,13 +4257,13 @@
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>149</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>109</v>
@@ -4284,13 +4280,13 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>109</v>
@@ -4446,8 +4442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4463,39 +4459,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="50" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B1" s="48" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C1" s="48" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D1" s="48" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E1" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="F1" s="48" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" s="49" t="s">
         <v>232</v>
-      </c>
-      <c r="F1" s="48" t="s">
-        <v>240</v>
-      </c>
-      <c r="G1" s="49" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="C2" s="44">
         <v>3</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E2" s="41">
         <v>0</v>
@@ -4508,7 +4504,7 @@
       <c r="B3" s="20"/>
       <c r="C3" s="45"/>
       <c r="D3" s="28" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E3" s="42">
         <v>1</v>
@@ -4521,7 +4517,7 @@
       <c r="B4" s="20"/>
       <c r="C4" s="45"/>
       <c r="D4" s="28" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E4" s="42">
         <v>2</v>
@@ -4534,7 +4530,7 @@
       <c r="B5" s="20"/>
       <c r="C5" s="45"/>
       <c r="D5" s="28" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E5" s="42">
         <v>3</v>
@@ -4547,7 +4543,7 @@
       <c r="B6" s="20"/>
       <c r="C6" s="45"/>
       <c r="D6" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E6" s="42">
         <v>4</v>
@@ -4560,7 +4556,7 @@
       <c r="B7" s="20"/>
       <c r="C7" s="45"/>
       <c r="D7" s="28" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E7" s="42">
         <v>5</v>
@@ -4573,7 +4569,7 @@
       <c r="B8" s="20"/>
       <c r="C8" s="45"/>
       <c r="D8" s="28" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E8" s="42">
         <v>6</v>
@@ -4586,7 +4582,7 @@
       <c r="B9" s="25"/>
       <c r="C9" s="46"/>
       <c r="D9" s="24" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E9" s="43">
         <v>7</v>
@@ -4596,16 +4592,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="51" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="C10" s="44">
         <v>3</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E10" s="41">
         <v>0</v>
@@ -4618,7 +4614,7 @@
       <c r="B11" s="20"/>
       <c r="C11" s="45"/>
       <c r="D11" s="28" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E11" s="42">
         <v>1</v>
@@ -4631,7 +4627,7 @@
       <c r="B12" s="20"/>
       <c r="C12" s="45"/>
       <c r="D12" s="28" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E12" s="42">
         <v>2</v>
@@ -4644,7 +4640,7 @@
       <c r="B13" s="20"/>
       <c r="C13" s="45"/>
       <c r="D13" s="28" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="E13" s="42">
         <v>3</v>
@@ -4657,7 +4653,7 @@
       <c r="B14" s="20"/>
       <c r="C14" s="45"/>
       <c r="D14" s="28" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E14" s="42">
         <v>4</v>
@@ -4670,7 +4666,7 @@
       <c r="B15" s="20"/>
       <c r="C15" s="45"/>
       <c r="D15" s="28" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E15" s="42">
         <v>5</v>
@@ -4683,7 +4679,7 @@
       <c r="B16" s="20"/>
       <c r="C16" s="45"/>
       <c r="D16" s="28" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E16" s="42">
         <v>6</v>
@@ -4696,7 +4692,7 @@
       <c r="B17" s="25"/>
       <c r="C17" s="46"/>
       <c r="D17" s="24" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="E17" s="43">
         <v>7</v>
@@ -4706,10 +4702,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="51" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C18" s="44">
         <v>6</v>
@@ -4725,18 +4721,18 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="52" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C19" s="45">
         <v>6</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="42"/>
-      <c r="F19" s="45">
-        <v>-31</v>
+      <c r="F19" s="45" t="s">
+        <v>310</v>
       </c>
       <c r="G19" s="42">
         <v>32</v>
@@ -4744,10 +4740,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="52" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C20" s="45">
         <v>8</v>
@@ -4763,10 +4759,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="52" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C21" s="45">
         <v>8</v>
@@ -4782,10 +4778,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="52" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C22" s="45">
         <v>12</v>
@@ -4801,10 +4797,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="C23" s="46">
         <v>12</v>
@@ -4820,16 +4816,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C24" s="44">
         <v>1</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E24" s="41">
         <v>0</v>
@@ -4842,7 +4838,7 @@
       <c r="B25" s="25"/>
       <c r="C25" s="46"/>
       <c r="D25" s="24" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E25" s="43">
         <v>1</v>
@@ -4852,16 +4848,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C26" s="44">
         <v>3</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="E26" s="41">
         <v>0</v>
@@ -4874,7 +4870,7 @@
       <c r="B27" s="20"/>
       <c r="C27" s="45"/>
       <c r="D27" s="28" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E27" s="42">
         <v>1</v>
@@ -4887,7 +4883,7 @@
       <c r="B28" s="20"/>
       <c r="C28" s="45"/>
       <c r="D28" s="28" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E28" s="42">
         <v>2</v>
@@ -4900,7 +4896,7 @@
       <c r="B29" s="20"/>
       <c r="C29" s="45"/>
       <c r="D29" s="28" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="E29" s="42">
         <v>3</v>
@@ -4913,7 +4909,7 @@
       <c r="B30" s="20"/>
       <c r="C30" s="45"/>
       <c r="D30" s="28" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E30" s="42">
         <v>4</v>
@@ -4926,7 +4922,7 @@
       <c r="B31" s="20"/>
       <c r="C31" s="45"/>
       <c r="D31" s="28" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E31" s="42">
         <v>5</v>
@@ -4939,7 +4935,7 @@
       <c r="B32" s="25"/>
       <c r="C32" s="46"/>
       <c r="D32" s="24" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="E32" s="43">
         <v>6</v>
@@ -4949,16 +4945,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="51" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C33" s="44">
         <v>3</v>
       </c>
       <c r="D33" s="22" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="E33" s="41">
         <v>0</v>
@@ -4971,7 +4967,7 @@
       <c r="B34" s="20"/>
       <c r="C34" s="45"/>
       <c r="D34" s="28" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="E34" s="42">
         <v>1</v>
@@ -4984,7 +4980,7 @@
       <c r="B35" s="20"/>
       <c r="C35" s="45"/>
       <c r="D35" s="28" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="E35" s="42">
         <v>2</v>
@@ -4997,7 +4993,7 @@
       <c r="B36" s="20"/>
       <c r="C36" s="45"/>
       <c r="D36" s="28" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="E36" s="42">
         <v>3</v>
@@ -5010,7 +5006,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="45"/>
       <c r="D37" s="28" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="E37" s="42">
         <v>4</v>
@@ -5023,7 +5019,7 @@
       <c r="B38" s="20"/>
       <c r="C38" s="45"/>
       <c r="D38" s="28" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="E38" s="42">
         <v>5</v>
@@ -5036,7 +5032,7 @@
       <c r="B39" s="25"/>
       <c r="C39" s="46"/>
       <c r="D39" s="24" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="E39" s="43">
         <v>6</v>
@@ -5046,7 +5042,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="54" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B40" s="31"/>
       <c r="C40" s="47"/>
@@ -5146,7 +5142,7 @@
         <v>105</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>12</v>
@@ -5190,7 +5186,7 @@
         <v>114</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>22</v>
@@ -5300,7 +5296,7 @@
         <v>153</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>96</v>
@@ -5407,13 +5403,13 @@
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5429,13 +5425,13 @@
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5460,13 +5456,13 @@
     </row>
     <row r="36" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5482,24 +5478,24 @@
     </row>
     <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>86</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>87</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5515,13 +5511,13 @@
     </row>
     <row r="41" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5532,18 +5528,18 @@
         <v>51</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>136</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5559,156 +5555,156 @@
     </row>
     <row r="45" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>137</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>139</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>140</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>110</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>144</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>143</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>142</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="11" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>145</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>146</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>147</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>148</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>149</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="11" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>150</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
all microfunctions get address
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="317">
   <si>
     <t>Instruction</t>
   </si>
@@ -975,6 +975,9 @@
   </si>
   <si>
     <t>DST = DST + DST</t>
+  </si>
+  <si>
+    <t>rrr0</t>
   </si>
 </sst>
 </file>
@@ -1799,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,8 +2960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E48" sqref="E47:E48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3012,7 +3015,7 @@
         <v>100</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3064,7 +3067,7 @@
         <v>100</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3087,7 +3090,7 @@
         <v>100</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3168,7 +3171,7 @@
         <v>100</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3191,7 +3194,7 @@
         <v>100</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3272,7 +3275,7 @@
         <v>100</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3295,7 +3298,7 @@
         <v>100</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>104</v>
@@ -3324,7 +3327,7 @@
         <v>100</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3376,7 +3379,7 @@
         <v>100</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3428,7 +3431,7 @@
         <v>100</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3451,7 +3454,7 @@
         <v>100</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3560,7 +3563,7 @@
         <v>112</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>101</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3757,7 +3760,7 @@
         <v>103</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>104</v>

</xml_diff>

<commit_message>
fixed operands input bus
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="348">
   <si>
     <t>Instruction</t>
   </si>
@@ -1068,6 +1068,9 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>ANDI DST, IMM8</t>
   </si>
 </sst>
 </file>
@@ -1895,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B26:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2098,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="38" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="B13" s="32" t="s">
         <v>180</v>
@@ -3075,8 +3078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3661,7 +3664,7 @@
         <v>112</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>291</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4558,10 +4561,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5000,10 +5003,10 @@
       <c r="B25" s="25"/>
       <c r="C25" s="46"/>
       <c r="D25" s="53"/>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="F25" s="42" t="s">
+      <c r="F25" s="43" t="s">
         <v>306</v>
       </c>
       <c r="G25" s="25"/>
@@ -5020,12 +5023,12 @@
         <v>3</v>
       </c>
       <c r="D26" s="52" t="s">
-        <v>343</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>333</v>
-      </c>
-      <c r="F26" s="41" t="s">
+        <v>346</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="F26" s="42" t="s">
         <v>295</v>
       </c>
       <c r="G26" s="18"/>
@@ -5035,14 +5038,12 @@
       <c r="A27" s="52"/>
       <c r="B27" s="20"/>
       <c r="C27" s="45"/>
-      <c r="D27" s="52" t="s">
-        <v>346</v>
-      </c>
+      <c r="D27" s="52"/>
       <c r="E27" s="28" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="29"/>
@@ -5053,10 +5054,10 @@
       <c r="C28" s="45"/>
       <c r="D28" s="52"/>
       <c r="E28" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="29"/>
@@ -5067,10 +5068,10 @@
       <c r="C29" s="45"/>
       <c r="D29" s="52"/>
       <c r="E29" s="28" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="29"/>
@@ -5081,10 +5082,10 @@
       <c r="C30" s="45"/>
       <c r="D30" s="52"/>
       <c r="E30" s="28" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="29"/>
@@ -5095,10 +5096,10 @@
       <c r="C31" s="45"/>
       <c r="D31" s="52"/>
       <c r="E31" s="28" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F31" s="42" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="29"/>
@@ -5109,10 +5110,10 @@
       <c r="C32" s="45"/>
       <c r="D32" s="52"/>
       <c r="E32" s="28" t="s">
-        <v>230</v>
+        <v>293</v>
       </c>
       <c r="F32" s="42" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="29"/>
@@ -5121,50 +5122,51 @@
       <c r="A33" s="52"/>
       <c r="B33" s="20"/>
       <c r="C33" s="45"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="28" t="s">
-        <v>293</v>
-      </c>
-      <c r="F33" s="42" t="s">
-        <v>307</v>
+      <c r="D33" s="53"/>
+      <c r="E33" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>297</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="29"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="25"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="F34" s="43" t="s">
-        <v>297</v>
-      </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="27"/>
+      <c r="A34" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="C34" s="44">
+        <v>3</v>
+      </c>
+      <c r="D34" s="52" t="s">
+        <v>346</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="F34" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="G34" s="18"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>241</v>
-      </c>
-      <c r="C35" s="44">
-        <v>3</v>
-      </c>
-      <c r="D35" s="52" t="s">
-        <v>346</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="F35" s="41" t="s">
-        <v>295</v>
-      </c>
-      <c r="G35" s="18"/>
-      <c r="H35" s="23"/>
+      <c r="A35" s="52"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>296</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="29"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="52"/>
@@ -5172,10 +5174,10 @@
       <c r="C36" s="45"/>
       <c r="D36" s="52"/>
       <c r="E36" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="29"/>
@@ -5186,10 +5188,10 @@
       <c r="C37" s="45"/>
       <c r="D37" s="52"/>
       <c r="E37" s="28" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="F37" s="42" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="29"/>
@@ -5200,10 +5202,10 @@
       <c r="C38" s="45"/>
       <c r="D38" s="52"/>
       <c r="E38" s="28" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F38" s="42" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="29"/>
@@ -5214,10 +5216,10 @@
       <c r="C39" s="45"/>
       <c r="D39" s="52"/>
       <c r="E39" s="28" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F39" s="42" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="29"/>
@@ -5228,63 +5230,57 @@
       <c r="C40" s="45"/>
       <c r="D40" s="52"/>
       <c r="E40" s="28" t="s">
-        <v>230</v>
+        <v>293</v>
       </c>
       <c r="F40" s="42" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="29"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="45"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="28" t="s">
-        <v>293</v>
-      </c>
-      <c r="F41" s="42" t="s">
-        <v>307</v>
-      </c>
-      <c r="G41" s="20"/>
-      <c r="H41" s="29"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>297</v>
+      </c>
+      <c r="G41" s="25"/>
+      <c r="H41" s="27"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="53"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="F42" s="43" t="s">
-        <v>297</v>
-      </c>
-      <c r="G42" s="25"/>
-      <c r="H42" s="27"/>
+      <c r="A42" s="54" t="s">
+        <v>231</v>
+      </c>
+      <c r="B42" s="31"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="33"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="54" t="s">
-        <v>231</v>
+        <v>333</v>
       </c>
       <c r="B43" s="31"/>
       <c r="C43" s="47"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="61"/>
+      <c r="D43" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="F43" s="61" t="s">
+        <v>295</v>
+      </c>
       <c r="G43" s="31"/>
       <c r="H43" s="33"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="45"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed typo in encoding file
</commit_message>
<xml_diff>
--- a/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
+++ b/HasmParser/Resources/Instructionset with Encoding (rev3).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11490" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MicroInstructions" sheetId="3" r:id="rId1"/>
@@ -1898,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B26:B27"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3078,8 +3078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:B60"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>26</v>
@@ -4563,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>